<commit_message>
Added images for tutorial activities in week 8
</commit_message>
<xml_diff>
--- a/src/tutorialpkg/data_db_activity/paralympics_all.xlsx
+++ b/src/tutorialpkg/data_db_activity/paralympics_all.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/comp0035-2024-tutorials/src/tutorialpkg/data_db_activity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19D8FBA-059A-E845-9A84-9795E84889C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9967DB-F9CE-D748-A176-35C2C6EDB219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32020" yWindow="2420" windowWidth="28040" windowHeight="17200" activeTab="2" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3827" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3827" uniqueCount="623">
   <si>
     <t>type</t>
   </si>
@@ -1140,9 +1140,6 @@
   </si>
   <si>
     <t>First summer games in France. The first time the Paralympic Opening Ceremony was held outside of a stadium</t>
-  </si>
-  <si>
-    <t>Summer</t>
   </si>
   <si>
     <t xml:space="preserve">winter </t>
@@ -2797,8 +2794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A5B346-9586-614E-9210-4DD6279EFFF5}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2829,7 +2826,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -2853,12 +2850,12 @@
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>367</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>1960</v>
@@ -3140,10 +3137,10 @@
         <v>1984</v>
       </c>
       <c r="C8" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E8" s="1">
         <v>30850</v>
@@ -3680,7 +3677,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B20">
         <v>1976</v>
@@ -28072,7 +28069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F26787-32FA-BD41-A79F-E693C34EE735}">
   <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28086,36 +28083,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>620</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>621</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" t="s">
         <v>370</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>371</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>372</v>
-      </c>
-      <c r="D2" t="s">
-        <v>373</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -28123,16 +28120,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B3" t="s">
         <v>374</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>375</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>376</v>
-      </c>
-      <c r="D3" t="s">
-        <v>377</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -28146,10 +28143,10 @@
         <v>242</v>
       </c>
       <c r="C4" t="s">
+        <v>377</v>
+      </c>
+      <c r="D4" t="s">
         <v>378</v>
-      </c>
-      <c r="D4" t="s">
-        <v>379</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -28157,16 +28154,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" t="s">
         <v>380</v>
       </c>
-      <c r="B5" t="s">
-        <v>381</v>
-      </c>
       <c r="C5" t="s">
+        <v>375</v>
+      </c>
+      <c r="D5" t="s">
         <v>376</v>
-      </c>
-      <c r="D5" t="s">
-        <v>377</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -28180,10 +28177,10 @@
         <v>274</v>
       </c>
       <c r="C6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -28191,16 +28188,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B7" t="s">
         <v>383</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>384</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>385</v>
-      </c>
-      <c r="D7" t="s">
-        <v>386</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
@@ -28214,10 +28211,10 @@
         <v>134</v>
       </c>
       <c r="C8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D8" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
@@ -28225,16 +28222,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B9" t="s">
         <v>388</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>375</v>
+      </c>
+      <c r="D9" t="s">
         <v>389</v>
-      </c>
-      <c r="C9" t="s">
-        <v>376</v>
-      </c>
-      <c r="D9" t="s">
-        <v>390</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -28242,16 +28239,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" t="s">
         <v>391</v>
       </c>
-      <c r="B10" t="s">
-        <v>392</v>
-      </c>
       <c r="C10" t="s">
+        <v>384</v>
+      </c>
+      <c r="D10" t="s">
         <v>385</v>
-      </c>
-      <c r="D10" t="s">
-        <v>386</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -28259,16 +28256,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B11" t="s">
         <v>393</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>394</v>
       </c>
-      <c r="C11" t="s">
-        <v>395</v>
-      </c>
       <c r="D11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
@@ -28282,10 +28279,10 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
@@ -28299,10 +28296,10 @@
         <v>69</v>
       </c>
       <c r="C13" t="s">
+        <v>375</v>
+      </c>
+      <c r="D13" t="s">
         <v>376</v>
-      </c>
-      <c r="D13" t="s">
-        <v>377</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
@@ -28316,10 +28313,10 @@
         <v>261</v>
       </c>
       <c r="C14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
@@ -28327,16 +28324,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B15" t="s">
         <v>396</v>
       </c>
-      <c r="B15" t="s">
-        <v>397</v>
-      </c>
       <c r="C15" t="s">
+        <v>384</v>
+      </c>
+      <c r="D15" t="s">
         <v>385</v>
-      </c>
-      <c r="D15" t="s">
-        <v>386</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -28344,16 +28341,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B16" t="s">
         <v>398</v>
       </c>
-      <c r="B16" t="s">
-        <v>399</v>
-      </c>
       <c r="C16" t="s">
+        <v>371</v>
+      </c>
+      <c r="D16" t="s">
         <v>372</v>
-      </c>
-      <c r="D16" t="s">
-        <v>373</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
@@ -28361,16 +28358,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B17" t="s">
         <v>400</v>
       </c>
-      <c r="B17" t="s">
-        <v>401</v>
-      </c>
       <c r="C17" t="s">
+        <v>384</v>
+      </c>
+      <c r="D17" t="s">
         <v>385</v>
-      </c>
-      <c r="D17" t="s">
-        <v>386</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -28378,16 +28375,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="B18" t="s">
         <v>402</v>
       </c>
-      <c r="B18" t="s">
-        <v>403</v>
-      </c>
       <c r="C18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E18" t="s">
         <v>2</v>
@@ -28401,10 +28398,10 @@
         <v>136</v>
       </c>
       <c r="C19" t="s">
+        <v>375</v>
+      </c>
+      <c r="D19" t="s">
         <v>376</v>
-      </c>
-      <c r="D19" t="s">
-        <v>377</v>
       </c>
       <c r="E19" t="s">
         <v>2</v>
@@ -28412,16 +28409,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="B20" t="s">
         <v>404</v>
       </c>
-      <c r="B20" t="s">
-        <v>405</v>
-      </c>
       <c r="C20" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D20" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
@@ -28429,16 +28426,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B21" t="s">
         <v>406</v>
       </c>
-      <c r="B21" t="s">
-        <v>407</v>
-      </c>
       <c r="C21" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E21" t="s">
         <v>2</v>
@@ -28446,16 +28443,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B22" t="s">
         <v>408</v>
       </c>
-      <c r="B22" t="s">
-        <v>409</v>
-      </c>
       <c r="C22" t="s">
+        <v>371</v>
+      </c>
+      <c r="D22" t="s">
         <v>372</v>
-      </c>
-      <c r="D22" t="s">
-        <v>373</v>
       </c>
       <c r="E22" t="s">
         <v>2</v>
@@ -28469,10 +28466,10 @@
         <v>263</v>
       </c>
       <c r="C23" t="s">
+        <v>375</v>
+      </c>
+      <c r="D23" t="s">
         <v>376</v>
-      </c>
-      <c r="D23" t="s">
-        <v>377</v>
       </c>
       <c r="E23" t="s">
         <v>2</v>
@@ -28480,16 +28477,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B24" t="s">
         <v>410</v>
       </c>
-      <c r="B24" t="s">
-        <v>411</v>
-      </c>
       <c r="C24" t="s">
+        <v>384</v>
+      </c>
+      <c r="D24" t="s">
         <v>385</v>
-      </c>
-      <c r="D24" t="s">
-        <v>386</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
@@ -28503,10 +28500,10 @@
         <v>236</v>
       </c>
       <c r="C25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D25" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E25" t="s">
         <v>2</v>
@@ -28514,16 +28511,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="B26" t="s">
         <v>412</v>
       </c>
-      <c r="B26" t="s">
-        <v>413</v>
-      </c>
       <c r="C26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E26" t="s">
         <v>2</v>
@@ -28537,10 +28534,10 @@
         <v>280</v>
       </c>
       <c r="C27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
@@ -28554,10 +28551,10 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E28" t="s">
         <v>2</v>
@@ -28571,10 +28568,10 @@
         <v>160</v>
       </c>
       <c r="C29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E29" t="s">
         <v>2</v>
@@ -28582,16 +28579,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B30" t="s">
         <v>415</v>
       </c>
-      <c r="B30" t="s">
-        <v>416</v>
-      </c>
       <c r="C30" t="s">
+        <v>371</v>
+      </c>
+      <c r="D30" t="s">
         <v>372</v>
-      </c>
-      <c r="D30" t="s">
-        <v>373</v>
       </c>
       <c r="E30" t="s">
         <v>2</v>
@@ -28605,10 +28602,10 @@
         <v>162</v>
       </c>
       <c r="C31" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D31" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E31" t="s">
         <v>2</v>
@@ -28616,36 +28613,36 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B32" t="s">
         <v>417</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>377</v>
+      </c>
+      <c r="D32" t="s">
+        <v>381</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>418</v>
-      </c>
-      <c r="C32" t="s">
-        <v>378</v>
-      </c>
-      <c r="D32" t="s">
-        <v>382</v>
-      </c>
-      <c r="E32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B33" t="s">
         <v>420</v>
       </c>
-      <c r="B33" t="s">
-        <v>421</v>
-      </c>
       <c r="C33" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D33" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E33" t="s">
         <v>2</v>
@@ -28653,16 +28650,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B34" t="s">
         <v>422</v>
       </c>
-      <c r="B34" t="s">
-        <v>423</v>
-      </c>
       <c r="C34" t="s">
+        <v>371</v>
+      </c>
+      <c r="D34" t="s">
         <v>372</v>
-      </c>
-      <c r="D34" t="s">
-        <v>373</v>
       </c>
       <c r="E34" t="s">
         <v>2</v>
@@ -28676,10 +28673,10 @@
         <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D35" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E35" t="s">
         <v>2</v>
@@ -28687,16 +28684,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B36" t="s">
         <v>424</v>
       </c>
-      <c r="B36" t="s">
-        <v>425</v>
-      </c>
       <c r="C36" t="s">
+        <v>384</v>
+      </c>
+      <c r="D36" t="s">
         <v>385</v>
-      </c>
-      <c r="D36" t="s">
-        <v>386</v>
       </c>
       <c r="E36" t="s">
         <v>2</v>
@@ -28704,36 +28701,36 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B37" t="s">
         <v>426</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>377</v>
+      </c>
+      <c r="D37" t="s">
+        <v>381</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>427</v>
-      </c>
-      <c r="C37" t="s">
-        <v>378</v>
-      </c>
-      <c r="D37" t="s">
-        <v>382</v>
-      </c>
-      <c r="E37" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B38" t="s">
         <v>429</v>
       </c>
-      <c r="B38" t="s">
-        <v>430</v>
-      </c>
       <c r="C38" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D38" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E38" t="s">
         <v>2</v>
@@ -28747,10 +28744,10 @@
         <v>310</v>
       </c>
       <c r="C39" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D39" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E39" t="s">
         <v>2</v>
@@ -28764,10 +28761,10 @@
         <v>157</v>
       </c>
       <c r="C40" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D40" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E40" t="s">
         <v>2</v>
@@ -28778,13 +28775,13 @@
         <v>246</v>
       </c>
       <c r="B41" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C41" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D41" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E41" t="s">
         <v>2</v>
@@ -28792,16 +28789,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B42" t="s">
         <v>433</v>
       </c>
-      <c r="B42" t="s">
-        <v>434</v>
-      </c>
       <c r="C42" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D42" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E42" t="s">
         <v>2</v>
@@ -28809,16 +28806,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B43" t="s">
         <v>435</v>
       </c>
-      <c r="B43" t="s">
-        <v>436</v>
-      </c>
       <c r="C43" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D43" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E43" t="s">
         <v>2</v>
@@ -28826,16 +28823,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="B44" t="s">
         <v>437</v>
       </c>
-      <c r="B44" t="s">
-        <v>438</v>
-      </c>
       <c r="C44" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D44" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E44" t="s">
         <v>2</v>
@@ -28849,10 +28846,10 @@
         <v>153</v>
       </c>
       <c r="C45" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D45" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E45" t="s">
         <v>2</v>
@@ -28860,16 +28857,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="B46" t="s">
         <v>439</v>
       </c>
-      <c r="B46" t="s">
-        <v>440</v>
-      </c>
       <c r="C46" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D46" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E46" t="s">
         <v>2</v>
@@ -28883,10 +28880,10 @@
         <v>332</v>
       </c>
       <c r="C47" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D47" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E47" t="s">
         <v>2</v>
@@ -28900,10 +28897,10 @@
         <v>336</v>
       </c>
       <c r="C48" t="s">
+        <v>384</v>
+      </c>
+      <c r="D48" t="s">
         <v>385</v>
-      </c>
-      <c r="D48" t="s">
-        <v>386</v>
       </c>
       <c r="E48" t="s">
         <v>2</v>
@@ -28917,10 +28914,10 @@
         <v>227</v>
       </c>
       <c r="C49" t="s">
+        <v>375</v>
+      </c>
+      <c r="D49" t="s">
         <v>376</v>
-      </c>
-      <c r="D49" t="s">
-        <v>377</v>
       </c>
       <c r="E49" t="s">
         <v>2</v>
@@ -28934,10 +28931,10 @@
         <v>197</v>
       </c>
       <c r="C50" t="s">
+        <v>384</v>
+      </c>
+      <c r="D50" t="s">
         <v>385</v>
-      </c>
-      <c r="D50" t="s">
-        <v>386</v>
       </c>
       <c r="E50" t="s">
         <v>2</v>
@@ -28945,16 +28942,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="B51" t="s">
         <v>441</v>
       </c>
-      <c r="B51" t="s">
-        <v>442</v>
-      </c>
       <c r="C51" t="s">
+        <v>384</v>
+      </c>
+      <c r="D51" t="s">
         <v>385</v>
-      </c>
-      <c r="D51" t="s">
-        <v>386</v>
       </c>
       <c r="E51" t="s">
         <v>2</v>
@@ -28968,10 +28965,10 @@
         <v>282</v>
       </c>
       <c r="C52" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D52" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E52" t="s">
         <v>2</v>
@@ -28985,16 +28982,16 @@
         <v>238</v>
       </c>
       <c r="C53" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D53" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E53" t="s">
         <v>2</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -29005,10 +29002,10 @@
         <v>149</v>
       </c>
       <c r="C54" t="s">
+        <v>375</v>
+      </c>
+      <c r="D54" t="s">
         <v>376</v>
-      </c>
-      <c r="D54" t="s">
-        <v>377</v>
       </c>
       <c r="E54" t="s">
         <v>2</v>
@@ -29016,16 +29013,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B55" t="s">
         <v>444</v>
       </c>
-      <c r="B55" t="s">
-        <v>445</v>
-      </c>
       <c r="C55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D55" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E55" t="s">
         <v>2</v>
@@ -29033,16 +29030,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B56" t="s">
         <v>446</v>
       </c>
-      <c r="B56" t="s">
-        <v>447</v>
-      </c>
       <c r="C56" t="s">
+        <v>384</v>
+      </c>
+      <c r="D56" t="s">
         <v>385</v>
-      </c>
-      <c r="D56" t="s">
-        <v>386</v>
       </c>
       <c r="E56" t="s">
         <v>2</v>
@@ -29056,10 +29053,10 @@
         <v>249</v>
       </c>
       <c r="C57" t="s">
+        <v>384</v>
+      </c>
+      <c r="D57" t="s">
         <v>385</v>
-      </c>
-      <c r="D57" t="s">
-        <v>386</v>
       </c>
       <c r="E57" t="s">
         <v>2</v>
@@ -29073,10 +29070,10 @@
         <v>338</v>
       </c>
       <c r="C58" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D58" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E58" t="s">
         <v>2</v>
@@ -29090,10 +29087,10 @@
         <v>148</v>
       </c>
       <c r="C59" t="s">
+        <v>377</v>
+      </c>
+      <c r="D59" t="s">
         <v>378</v>
-      </c>
-      <c r="D59" t="s">
-        <v>379</v>
       </c>
       <c r="E59" t="s">
         <v>2</v>
@@ -29101,16 +29098,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="B60" t="s">
         <v>448</v>
       </c>
-      <c r="B60" t="s">
-        <v>449</v>
-      </c>
       <c r="C60" t="s">
+        <v>375</v>
+      </c>
+      <c r="D60" t="s">
         <v>376</v>
-      </c>
-      <c r="D60" t="s">
-        <v>377</v>
       </c>
       <c r="E60" t="s">
         <v>2</v>
@@ -29118,16 +29115,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="B61" t="s">
         <v>450</v>
       </c>
-      <c r="B61" t="s">
-        <v>451</v>
-      </c>
       <c r="C61" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D61" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E61" t="s">
         <v>2</v>
@@ -29141,10 +29138,10 @@
         <v>340</v>
       </c>
       <c r="C62" t="s">
+        <v>384</v>
+      </c>
+      <c r="D62" t="s">
         <v>385</v>
-      </c>
-      <c r="D62" t="s">
-        <v>386</v>
       </c>
       <c r="E62" t="s">
         <v>2</v>
@@ -29158,10 +29155,10 @@
         <v>38</v>
       </c>
       <c r="C63" t="s">
+        <v>375</v>
+      </c>
+      <c r="D63" t="s">
         <v>376</v>
-      </c>
-      <c r="D63" t="s">
-        <v>377</v>
       </c>
       <c r="E63" t="s">
         <v>2</v>
@@ -29175,10 +29172,10 @@
         <v>217</v>
       </c>
       <c r="C64" t="s">
+        <v>375</v>
+      </c>
+      <c r="D64" t="s">
         <v>376</v>
-      </c>
-      <c r="D64" t="s">
-        <v>377</v>
       </c>
       <c r="E64" t="s">
         <v>2</v>
@@ -29192,10 +29189,10 @@
         <v>314</v>
       </c>
       <c r="C65" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D65" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E65" t="s">
         <v>2</v>
@@ -29203,19 +29200,19 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B66" t="s">
         <v>452</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>375</v>
+      </c>
+      <c r="D66" t="s">
+        <v>376</v>
+      </c>
+      <c r="E66" t="s">
         <v>453</v>
-      </c>
-      <c r="C66" t="s">
-        <v>376</v>
-      </c>
-      <c r="D66" t="s">
-        <v>377</v>
-      </c>
-      <c r="E66" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -29226,10 +29223,10 @@
         <v>357</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -29240,10 +29237,10 @@
         <v>312</v>
       </c>
       <c r="C68" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D68" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E68" t="s">
         <v>2</v>
@@ -29257,10 +29254,10 @@
         <v>137</v>
       </c>
       <c r="C69" t="s">
+        <v>375</v>
+      </c>
+      <c r="D69" t="s">
         <v>376</v>
-      </c>
-      <c r="D69" t="s">
-        <v>377</v>
       </c>
       <c r="E69" t="s">
         <v>2</v>
@@ -29274,10 +29271,10 @@
         <v>59</v>
       </c>
       <c r="C70" t="s">
+        <v>375</v>
+      </c>
+      <c r="D70" t="s">
         <v>376</v>
-      </c>
-      <c r="D70" t="s">
-        <v>377</v>
       </c>
       <c r="E70" t="s">
         <v>2</v>
@@ -29291,10 +29288,10 @@
         <v>163</v>
       </c>
       <c r="C71" t="s">
+        <v>375</v>
+      </c>
+      <c r="D71" t="s">
         <v>376</v>
-      </c>
-      <c r="D71" t="s">
-        <v>377</v>
       </c>
       <c r="E71" t="s">
         <v>2</v>
@@ -29302,16 +29299,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B72" t="s">
         <v>456</v>
       </c>
-      <c r="B72" t="s">
-        <v>457</v>
-      </c>
       <c r="C72" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D72" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E72" t="s">
         <v>2</v>
@@ -29319,16 +29316,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="B73" t="s">
         <v>458</v>
       </c>
-      <c r="B73" t="s">
-        <v>459</v>
-      </c>
       <c r="C73" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D73" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E73" t="s">
         <v>2</v>
@@ -29336,16 +29333,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B74" t="s">
         <v>460</v>
       </c>
-      <c r="B74" t="s">
-        <v>461</v>
-      </c>
       <c r="C74" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D74" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E74" t="s">
         <v>2</v>
@@ -29359,10 +29356,10 @@
         <v>132</v>
       </c>
       <c r="C75" t="s">
+        <v>375</v>
+      </c>
+      <c r="D75" t="s">
         <v>376</v>
-      </c>
-      <c r="D75" t="s">
-        <v>377</v>
       </c>
       <c r="E75" t="s">
         <v>2</v>
@@ -29370,16 +29367,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B76" t="s">
         <v>462</v>
       </c>
-      <c r="B76" t="s">
-        <v>463</v>
-      </c>
       <c r="C76" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D76" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E76" t="s">
         <v>2</v>
@@ -29393,10 +29390,10 @@
         <v>326</v>
       </c>
       <c r="C77" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D77" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E77" t="s">
         <v>2</v>
@@ -29404,16 +29401,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B78" t="s">
         <v>464</v>
       </c>
-      <c r="B78" t="s">
-        <v>465</v>
-      </c>
       <c r="C78" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D78" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E78" t="s">
         <v>2</v>
@@ -29427,10 +29424,10 @@
         <v>24</v>
       </c>
       <c r="C79" t="s">
+        <v>375</v>
+      </c>
+      <c r="D79" t="s">
         <v>376</v>
-      </c>
-      <c r="D79" t="s">
-        <v>377</v>
       </c>
       <c r="E79" t="s">
         <v>2</v>
@@ -29438,16 +29435,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="B80" t="s">
         <v>466</v>
       </c>
-      <c r="B80" t="s">
-        <v>467</v>
-      </c>
       <c r="C80" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D80" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E80" t="s">
         <v>2</v>
@@ -29455,16 +29452,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="B81" t="s">
         <v>468</v>
       </c>
-      <c r="B81" t="s">
-        <v>469</v>
-      </c>
       <c r="C81" t="s">
+        <v>384</v>
+      </c>
+      <c r="D81" t="s">
         <v>385</v>
-      </c>
-      <c r="D81" t="s">
-        <v>386</v>
       </c>
       <c r="E81" t="s">
         <v>2</v>
@@ -29478,10 +29475,10 @@
         <v>48</v>
       </c>
       <c r="C82" t="s">
+        <v>375</v>
+      </c>
+      <c r="D82" t="s">
         <v>376</v>
-      </c>
-      <c r="D82" t="s">
-        <v>377</v>
       </c>
       <c r="E82" t="s">
         <v>2</v>
@@ -29489,16 +29486,16 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="B83" t="s">
         <v>470</v>
       </c>
-      <c r="B83" t="s">
-        <v>471</v>
-      </c>
       <c r="C83" t="s">
+        <v>384</v>
+      </c>
+      <c r="D83" t="s">
         <v>385</v>
-      </c>
-      <c r="D83" t="s">
-        <v>386</v>
       </c>
       <c r="E83" t="s">
         <v>2</v>
@@ -29506,16 +29503,16 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="B84" t="s">
         <v>472</v>
       </c>
-      <c r="B84" t="s">
-        <v>473</v>
-      </c>
       <c r="C84" t="s">
+        <v>384</v>
+      </c>
+      <c r="D84" t="s">
         <v>385</v>
-      </c>
-      <c r="D84" t="s">
-        <v>386</v>
       </c>
       <c r="E84" t="s">
         <v>2</v>
@@ -29523,16 +29520,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="B85" t="s">
         <v>474</v>
       </c>
-      <c r="B85" t="s">
-        <v>475</v>
-      </c>
       <c r="C85" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D85" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E85" t="s">
         <v>2</v>
@@ -29540,16 +29537,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B86" t="s">
         <v>476</v>
       </c>
-      <c r="B86" t="s">
-        <v>477</v>
-      </c>
       <c r="C86" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D86" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E86" t="s">
         <v>2</v>
@@ -29557,16 +29554,16 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="B87" t="s">
         <v>478</v>
       </c>
-      <c r="B87" t="s">
-        <v>479</v>
-      </c>
       <c r="C87" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D87" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E87" t="s">
         <v>2</v>
@@ -29574,16 +29571,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="B88" t="s">
         <v>480</v>
       </c>
-      <c r="B88" t="s">
-        <v>481</v>
-      </c>
       <c r="C88" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D88" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E88" t="s">
         <v>2</v>
@@ -29591,16 +29588,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B89" t="s">
         <v>482</v>
       </c>
-      <c r="B89" t="s">
-        <v>483</v>
-      </c>
       <c r="C89" t="s">
+        <v>384</v>
+      </c>
+      <c r="D89" t="s">
         <v>385</v>
-      </c>
-      <c r="D89" t="s">
-        <v>386</v>
       </c>
       <c r="E89" t="s">
         <v>2</v>
@@ -29614,10 +29611,10 @@
         <v>145</v>
       </c>
       <c r="C90" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D90" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E90" t="s">
         <v>2</v>
@@ -29625,16 +29622,16 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="B91" t="s">
         <v>484</v>
       </c>
-      <c r="B91" t="s">
-        <v>485</v>
-      </c>
       <c r="C91" t="s">
+        <v>384</v>
+      </c>
+      <c r="D91" t="s">
         <v>385</v>
-      </c>
-      <c r="D91" t="s">
-        <v>386</v>
       </c>
       <c r="E91" t="s">
         <v>2</v>
@@ -29648,10 +29645,10 @@
         <v>146</v>
       </c>
       <c r="C92" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D92" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E92" t="s">
         <v>2</v>
@@ -29665,10 +29662,10 @@
         <v>150</v>
       </c>
       <c r="C93" t="s">
+        <v>371</v>
+      </c>
+      <c r="D93" t="s">
         <v>372</v>
-      </c>
-      <c r="D93" t="s">
-        <v>373</v>
       </c>
       <c r="E93" t="s">
         <v>2</v>
@@ -29682,10 +29679,10 @@
         <v>143</v>
       </c>
       <c r="C94" t="s">
+        <v>371</v>
+      </c>
+      <c r="D94" t="s">
         <v>372</v>
-      </c>
-      <c r="D94" t="s">
-        <v>373</v>
       </c>
       <c r="E94" t="s">
         <v>2</v>
@@ -29693,16 +29690,16 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="B95" t="s">
         <v>486</v>
       </c>
-      <c r="B95" t="s">
-        <v>487</v>
-      </c>
       <c r="C95" t="s">
+        <v>375</v>
+      </c>
+      <c r="D95" t="s">
         <v>376</v>
-      </c>
-      <c r="D95" t="s">
-        <v>377</v>
       </c>
       <c r="E95" t="s">
         <v>2</v>
@@ -29710,22 +29707,22 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>488</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="C96" t="s">
+        <v>371</v>
+      </c>
+      <c r="D96" t="s">
+        <v>413</v>
+      </c>
+      <c r="E96" t="s">
         <v>489</v>
       </c>
-      <c r="C96" t="s">
-        <v>372</v>
-      </c>
-      <c r="D96" t="s">
-        <v>414</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="F96" s="5" t="s">
         <v>490</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -29736,10 +29733,10 @@
         <v>161</v>
       </c>
       <c r="C97" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D97" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E97" t="s">
         <v>2</v>
@@ -29753,10 +29750,10 @@
         <v>135</v>
       </c>
       <c r="C98" t="s">
+        <v>375</v>
+      </c>
+      <c r="D98" t="s">
         <v>376</v>
-      </c>
-      <c r="D98" t="s">
-        <v>377</v>
       </c>
       <c r="E98" t="s">
         <v>2</v>
@@ -29770,10 +29767,10 @@
         <v>229</v>
       </c>
       <c r="C99" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D99" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E99" t="s">
         <v>2</v>
@@ -29787,10 +29784,10 @@
         <v>154</v>
       </c>
       <c r="C100" t="s">
+        <v>375</v>
+      </c>
+      <c r="D100" t="s">
         <v>376</v>
-      </c>
-      <c r="D100" t="s">
-        <v>377</v>
       </c>
       <c r="E100" t="s">
         <v>2</v>
@@ -29804,10 +29801,10 @@
         <v>21</v>
       </c>
       <c r="C101" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D101" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E101" t="s">
         <v>2</v>
@@ -29815,16 +29812,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="B102" t="s">
         <v>492</v>
       </c>
-      <c r="B102" t="s">
-        <v>493</v>
-      </c>
       <c r="C102" t="s">
+        <v>384</v>
+      </c>
+      <c r="D102" t="s">
         <v>385</v>
-      </c>
-      <c r="D102" t="s">
-        <v>386</v>
       </c>
       <c r="E102" t="s">
         <v>2</v>
@@ -29838,10 +29835,10 @@
         <v>14</v>
       </c>
       <c r="C103" t="s">
+        <v>375</v>
+      </c>
+      <c r="D103" t="s">
         <v>376</v>
-      </c>
-      <c r="D103" t="s">
-        <v>377</v>
       </c>
       <c r="E103" t="s">
         <v>2</v>
@@ -29849,16 +29846,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="B104" t="s">
         <v>494</v>
       </c>
-      <c r="B104" t="s">
-        <v>495</v>
-      </c>
       <c r="C104" t="s">
+        <v>384</v>
+      </c>
+      <c r="D104" t="s">
         <v>385</v>
-      </c>
-      <c r="D104" t="s">
-        <v>386</v>
       </c>
       <c r="E104" t="s">
         <v>2</v>
@@ -29872,10 +29869,10 @@
         <v>139</v>
       </c>
       <c r="C105" t="s">
+        <v>384</v>
+      </c>
+      <c r="D105" t="s">
         <v>385</v>
-      </c>
-      <c r="D105" t="s">
-        <v>386</v>
       </c>
       <c r="E105" t="s">
         <v>2</v>
@@ -29889,10 +29886,10 @@
         <v>159</v>
       </c>
       <c r="C106" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D106" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E106" t="s">
         <v>2</v>
@@ -29906,10 +29903,10 @@
         <v>18</v>
       </c>
       <c r="C107" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D107" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E107" t="s">
         <v>2</v>
@@ -29923,10 +29920,10 @@
         <v>324</v>
       </c>
       <c r="C108" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D108" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E108" t="s">
         <v>2</v>
@@ -29940,10 +29937,10 @@
         <v>144</v>
       </c>
       <c r="C109" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D109" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E109" t="s">
         <v>2</v>
@@ -29951,16 +29948,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="B110" t="s">
         <v>496</v>
       </c>
-      <c r="B110" t="s">
-        <v>497</v>
-      </c>
       <c r="C110" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D110" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E110" t="s">
         <v>2</v>
@@ -29968,16 +29965,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="B111" t="s">
         <v>498</v>
       </c>
-      <c r="B111" t="s">
-        <v>499</v>
-      </c>
       <c r="C111" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D111" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E111" t="s">
         <v>2</v>
@@ -29991,10 +29988,10 @@
         <v>142</v>
       </c>
       <c r="C112" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D112" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E112" t="s">
         <v>2</v>
@@ -30002,16 +29999,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B113" t="s">
         <v>500</v>
       </c>
-      <c r="B113" t="s">
-        <v>501</v>
-      </c>
       <c r="C113" t="s">
+        <v>375</v>
+      </c>
+      <c r="D113" t="s">
         <v>376</v>
-      </c>
-      <c r="D113" t="s">
-        <v>377</v>
       </c>
       <c r="E113" t="s">
         <v>2</v>
@@ -30025,10 +30022,10 @@
         <v>355</v>
       </c>
       <c r="C114" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D114" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E114" t="s">
         <v>2</v>
@@ -30042,10 +30039,10 @@
         <v>152</v>
       </c>
       <c r="C115" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D115" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E115" t="s">
         <v>2</v>
@@ -30059,10 +30056,10 @@
         <v>304</v>
       </c>
       <c r="C116" t="s">
+        <v>371</v>
+      </c>
+      <c r="D116" t="s">
         <v>372</v>
-      </c>
-      <c r="D116" t="s">
-        <v>373</v>
       </c>
       <c r="E116" t="s">
         <v>2</v>
@@ -30076,10 +30073,10 @@
         <v>265</v>
       </c>
       <c r="C117" t="s">
+        <v>375</v>
+      </c>
+      <c r="D117" t="s">
         <v>376</v>
-      </c>
-      <c r="D117" t="s">
-        <v>377</v>
       </c>
       <c r="E117" t="s">
         <v>2</v>
@@ -30093,10 +30090,10 @@
         <v>267</v>
       </c>
       <c r="C118" t="s">
+        <v>377</v>
+      </c>
+      <c r="D118" t="s">
         <v>378</v>
-      </c>
-      <c r="D118" t="s">
-        <v>379</v>
       </c>
       <c r="E118" t="s">
         <v>2</v>
@@ -30110,10 +30107,10 @@
         <v>302</v>
       </c>
       <c r="C119" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D119" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E119" t="s">
         <v>2</v>
@@ -30121,16 +30118,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="B120" t="s">
         <v>502</v>
       </c>
-      <c r="B120" t="s">
-        <v>503</v>
-      </c>
       <c r="C120" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D120" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E120" t="s">
         <v>2</v>
@@ -30138,16 +30135,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="B121" t="s">
         <v>504</v>
       </c>
-      <c r="B121" t="s">
-        <v>505</v>
-      </c>
       <c r="C121" t="s">
+        <v>384</v>
+      </c>
+      <c r="D121" t="s">
         <v>385</v>
-      </c>
-      <c r="D121" t="s">
-        <v>386</v>
       </c>
       <c r="E121" t="s">
         <v>2</v>
@@ -30155,16 +30152,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="B122" t="s">
         <v>506</v>
       </c>
-      <c r="B122" t="s">
-        <v>507</v>
-      </c>
       <c r="C122" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D122" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E122" t="s">
         <v>2</v>
@@ -30178,10 +30175,10 @@
         <v>349</v>
       </c>
       <c r="C123" t="s">
+        <v>375</v>
+      </c>
+      <c r="D123" t="s">
         <v>376</v>
-      </c>
-      <c r="D123" t="s">
-        <v>377</v>
       </c>
       <c r="E123" t="s">
         <v>2</v>
@@ -30195,10 +30192,10 @@
         <v>214</v>
       </c>
       <c r="C124" t="s">
+        <v>375</v>
+      </c>
+      <c r="D124" t="s">
         <v>376</v>
-      </c>
-      <c r="D124" t="s">
-        <v>377</v>
       </c>
       <c r="E124" t="s">
         <v>2</v>
@@ -30206,16 +30203,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="B125" t="s">
         <v>508</v>
       </c>
-      <c r="B125" t="s">
-        <v>509</v>
-      </c>
       <c r="C125" t="s">
+        <v>375</v>
+      </c>
+      <c r="D125" t="s">
         <v>376</v>
-      </c>
-      <c r="D125" t="s">
-        <v>377</v>
       </c>
       <c r="E125" t="s">
         <v>2</v>
@@ -30223,16 +30220,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B126" t="s">
         <v>510</v>
       </c>
-      <c r="B126" t="s">
-        <v>511</v>
-      </c>
       <c r="C126" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D126" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E126" t="s">
         <v>2</v>
@@ -30240,16 +30237,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B127" t="s">
         <v>512</v>
       </c>
-      <c r="B127" t="s">
-        <v>513</v>
-      </c>
       <c r="C127" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D127" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E127" t="s">
         <v>2</v>
@@ -30263,10 +30260,10 @@
         <v>168</v>
       </c>
       <c r="C128" t="s">
+        <v>377</v>
+      </c>
+      <c r="D128" t="s">
         <v>378</v>
-      </c>
-      <c r="D128" t="s">
-        <v>379</v>
       </c>
       <c r="E128" t="s">
         <v>2</v>
@@ -30280,10 +30277,10 @@
         <v>167</v>
       </c>
       <c r="C129" t="s">
+        <v>371</v>
+      </c>
+      <c r="D129" t="s">
         <v>372</v>
-      </c>
-      <c r="D129" t="s">
-        <v>373</v>
       </c>
       <c r="E129" t="s">
         <v>2</v>
@@ -30291,16 +30288,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="B130" t="s">
         <v>514</v>
       </c>
-      <c r="B130" t="s">
-        <v>515</v>
-      </c>
       <c r="C130" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D130" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E130" t="s">
         <v>2</v>
@@ -30314,10 +30311,10 @@
         <v>254</v>
       </c>
       <c r="C131" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D131" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E131" t="s">
         <v>2</v>
@@ -30325,16 +30322,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="B132" t="s">
         <v>516</v>
       </c>
-      <c r="B132" t="s">
-        <v>517</v>
-      </c>
       <c r="C132" t="s">
+        <v>371</v>
+      </c>
+      <c r="D132" t="s">
         <v>372</v>
-      </c>
-      <c r="D132" t="s">
-        <v>373</v>
       </c>
       <c r="E132" t="s">
         <v>2</v>
@@ -30348,10 +30345,10 @@
         <v>147</v>
       </c>
       <c r="C133" t="s">
+        <v>384</v>
+      </c>
+      <c r="D133" t="s">
         <v>385</v>
-      </c>
-      <c r="D133" t="s">
-        <v>386</v>
       </c>
       <c r="E133" t="s">
         <v>2</v>
@@ -30365,10 +30362,10 @@
         <v>291</v>
       </c>
       <c r="C134" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D134" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E134" t="s">
         <v>2</v>
@@ -30376,16 +30373,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="B135" t="s">
         <v>518</v>
       </c>
-      <c r="B135" t="s">
-        <v>519</v>
-      </c>
       <c r="C135" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D135" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E135" t="s">
         <v>2</v>
@@ -30399,10 +30396,10 @@
         <v>284</v>
       </c>
       <c r="C136" t="s">
+        <v>375</v>
+      </c>
+      <c r="D136" t="s">
         <v>376</v>
-      </c>
-      <c r="D136" t="s">
-        <v>377</v>
       </c>
       <c r="E136" t="s">
         <v>2</v>
@@ -30410,16 +30407,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="B137" t="s">
         <v>520</v>
       </c>
-      <c r="B137" t="s">
-        <v>521</v>
-      </c>
       <c r="C137" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D137" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E137" t="s">
         <v>2</v>
@@ -30427,16 +30424,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="B138" t="s">
         <v>522</v>
       </c>
-      <c r="B138" t="s">
-        <v>523</v>
-      </c>
       <c r="C138" t="s">
+        <v>375</v>
+      </c>
+      <c r="D138" t="s">
         <v>376</v>
-      </c>
-      <c r="D138" t="s">
-        <v>377</v>
       </c>
       <c r="E138" t="s">
         <v>2</v>
@@ -30450,10 +30447,10 @@
         <v>342</v>
       </c>
       <c r="C139" t="s">
+        <v>375</v>
+      </c>
+      <c r="D139" t="s">
         <v>376</v>
-      </c>
-      <c r="D139" t="s">
-        <v>377</v>
       </c>
       <c r="E139" t="s">
         <v>2</v>
@@ -30461,16 +30458,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="B140" t="s">
         <v>524</v>
       </c>
-      <c r="B140" t="s">
-        <v>525</v>
-      </c>
       <c r="C140" t="s">
+        <v>375</v>
+      </c>
+      <c r="D140" t="s">
         <v>376</v>
-      </c>
-      <c r="D140" t="s">
-        <v>377</v>
       </c>
       <c r="E140" t="s">
         <v>2</v>
@@ -30484,10 +30481,10 @@
         <v>334</v>
       </c>
       <c r="C141" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D141" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E141" t="s">
         <v>2</v>
@@ -30495,16 +30492,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B142" t="s">
         <v>526</v>
       </c>
-      <c r="B142" t="s">
-        <v>527</v>
-      </c>
       <c r="C142" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D142" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E142" t="s">
         <v>2</v>
@@ -30512,16 +30509,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="B143" t="s">
         <v>528</v>
       </c>
-      <c r="B143" t="s">
-        <v>529</v>
-      </c>
       <c r="C143" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D143" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E143" t="s">
         <v>2</v>
@@ -30529,16 +30526,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="B144" t="s">
         <v>530</v>
       </c>
-      <c r="B144" t="s">
-        <v>531</v>
-      </c>
       <c r="C144" t="s">
+        <v>384</v>
+      </c>
+      <c r="D144" t="s">
         <v>385</v>
-      </c>
-      <c r="D144" t="s">
-        <v>386</v>
       </c>
       <c r="E144" t="s">
         <v>2</v>
@@ -30546,22 +30543,22 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="B145" t="s">
         <v>532</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" t="s">
+        <v>371</v>
+      </c>
+      <c r="D145" t="s">
+        <v>372</v>
+      </c>
+      <c r="E145" t="s">
+        <v>2</v>
+      </c>
+      <c r="F145" s="5" t="s">
         <v>533</v>
-      </c>
-      <c r="C145" t="s">
-        <v>372</v>
-      </c>
-      <c r="D145" t="s">
-        <v>373</v>
-      </c>
-      <c r="E145" t="s">
-        <v>2</v>
-      </c>
-      <c r="F145" s="5" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -30572,10 +30569,10 @@
         <v>306</v>
       </c>
       <c r="C146" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D146" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E146" t="s">
         <v>2</v>
@@ -30583,16 +30580,16 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B147" t="s">
         <v>535</v>
       </c>
-      <c r="B147" t="s">
-        <v>536</v>
-      </c>
       <c r="C147" t="s">
+        <v>384</v>
+      </c>
+      <c r="D147" t="s">
         <v>385</v>
-      </c>
-      <c r="D147" t="s">
-        <v>386</v>
       </c>
       <c r="E147" t="s">
         <v>2</v>
@@ -30600,16 +30597,16 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="B148" t="s">
         <v>537</v>
       </c>
-      <c r="B148" t="s">
-        <v>538</v>
-      </c>
       <c r="C148" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D148" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E148" t="s">
         <v>2</v>
@@ -30623,10 +30620,10 @@
         <v>31</v>
       </c>
       <c r="C149" t="s">
+        <v>375</v>
+      </c>
+      <c r="D149" t="s">
         <v>376</v>
-      </c>
-      <c r="D149" t="s">
-        <v>377</v>
       </c>
       <c r="E149" t="s">
         <v>2</v>
@@ -30634,16 +30631,16 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="B150" t="s">
         <v>539</v>
       </c>
-      <c r="B150" t="s">
-        <v>540</v>
-      </c>
       <c r="C150" t="s">
+        <v>371</v>
+      </c>
+      <c r="D150" t="s">
         <v>372</v>
-      </c>
-      <c r="D150" t="s">
-        <v>373</v>
       </c>
       <c r="E150" t="s">
         <v>2</v>
@@ -30657,10 +30654,10 @@
         <v>202</v>
       </c>
       <c r="C151" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D151" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E151" t="s">
         <v>2</v>
@@ -30668,16 +30665,16 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="B152" t="s">
         <v>541</v>
       </c>
-      <c r="B152" t="s">
-        <v>542</v>
-      </c>
       <c r="C152" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D152" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E152" t="s">
         <v>2</v>
@@ -30691,10 +30688,10 @@
         <v>66</v>
       </c>
       <c r="C153" t="s">
+        <v>375</v>
+      </c>
+      <c r="D153" t="s">
         <v>376</v>
-      </c>
-      <c r="D153" t="s">
-        <v>377</v>
       </c>
       <c r="E153" t="s">
         <v>2</v>
@@ -30708,27 +30705,27 @@
         <v>362</v>
       </c>
       <c r="C154" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D154" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E154" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="B155" t="s">
         <v>543</v>
       </c>
-      <c r="B155" t="s">
-        <v>544</v>
-      </c>
       <c r="C155" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D155" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E155" t="s">
         <v>2</v>
@@ -30742,10 +30739,10 @@
         <v>140</v>
       </c>
       <c r="C156" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D156" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E156" t="s">
         <v>2</v>
@@ -30759,10 +30756,10 @@
         <v>344</v>
       </c>
       <c r="C157" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D157" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E157" t="s">
         <v>2</v>
@@ -30776,10 +30773,10 @@
         <v>296</v>
       </c>
       <c r="C158" t="s">
+        <v>371</v>
+      </c>
+      <c r="D158" t="s">
         <v>372</v>
-      </c>
-      <c r="D158" t="s">
-        <v>373</v>
       </c>
       <c r="E158" t="s">
         <v>2</v>
@@ -30793,10 +30790,10 @@
         <v>210</v>
       </c>
       <c r="C159" t="s">
+        <v>384</v>
+      </c>
+      <c r="D159" t="s">
         <v>385</v>
-      </c>
-      <c r="D159" t="s">
-        <v>386</v>
       </c>
       <c r="E159" t="s">
         <v>2</v>
@@ -30804,16 +30801,16 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="B160" t="s">
         <v>545</v>
       </c>
-      <c r="B160" t="s">
-        <v>546</v>
-      </c>
       <c r="C160" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D160" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E160" t="s">
         <v>2</v>
@@ -30827,10 +30824,10 @@
         <v>151</v>
       </c>
       <c r="C161" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D161" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E161" t="s">
         <v>2</v>
@@ -30844,10 +30841,10 @@
         <v>271</v>
       </c>
       <c r="C162" t="s">
+        <v>371</v>
+      </c>
+      <c r="D162" t="s">
         <v>372</v>
-      </c>
-      <c r="D162" t="s">
-        <v>373</v>
       </c>
       <c r="E162" t="s">
         <v>2</v>
@@ -30861,10 +30858,10 @@
         <v>269</v>
       </c>
       <c r="C163" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D163" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E163" t="s">
         <v>2</v>
@@ -30872,16 +30869,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B164" t="s">
         <v>547</v>
       </c>
-      <c r="B164" t="s">
-        <v>548</v>
-      </c>
       <c r="C164" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D164" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E164" t="s">
         <v>2</v>
@@ -30895,10 +30892,10 @@
         <v>298</v>
       </c>
       <c r="C165" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D165" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E165" t="s">
         <v>2</v>
@@ -30912,10 +30909,10 @@
         <v>141</v>
       </c>
       <c r="C166" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D166" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E166" t="s">
         <v>2</v>
@@ -30929,10 +30926,10 @@
         <v>156</v>
       </c>
       <c r="C167" t="s">
+        <v>375</v>
+      </c>
+      <c r="D167" t="s">
         <v>376</v>
-      </c>
-      <c r="D167" t="s">
-        <v>377</v>
       </c>
       <c r="E167" t="s">
         <v>2</v>
@@ -30940,16 +30937,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="B168" t="s">
         <v>549</v>
       </c>
-      <c r="B168" t="s">
-        <v>550</v>
-      </c>
       <c r="C168" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D168" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E168" t="s">
         <v>2</v>
@@ -30963,10 +30960,10 @@
         <v>164</v>
       </c>
       <c r="C169" t="s">
+        <v>384</v>
+      </c>
+      <c r="D169" t="s">
         <v>385</v>
-      </c>
-      <c r="D169" t="s">
-        <v>386</v>
       </c>
       <c r="E169" t="s">
         <v>2</v>
@@ -30974,16 +30971,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="B170" t="s">
         <v>551</v>
       </c>
-      <c r="B170" t="s">
-        <v>552</v>
-      </c>
       <c r="C170" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D170" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E170" t="s">
         <v>2</v>
@@ -30997,10 +30994,10 @@
         <v>328</v>
       </c>
       <c r="C171" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D171" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E171" t="s">
         <v>2</v>
@@ -31014,10 +31011,10 @@
         <v>300</v>
       </c>
       <c r="C172" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D172" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E172" t="s">
         <v>2</v>
@@ -31031,30 +31028,30 @@
         <v>354</v>
       </c>
       <c r="C173" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D173" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E173" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="B174" t="s">
         <v>553</v>
       </c>
-      <c r="B174" t="s">
-        <v>554</v>
-      </c>
       <c r="C174" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D174" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E174" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -31065,10 +31062,10 @@
         <v>138</v>
       </c>
       <c r="C175" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D175" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E175" t="s">
         <v>2</v>
@@ -31076,19 +31073,19 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B176" t="s">
         <v>555</v>
       </c>
-      <c r="B176" t="s">
-        <v>556</v>
-      </c>
       <c r="C176" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D176" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E176" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -31099,10 +31096,10 @@
         <v>234</v>
       </c>
       <c r="C177" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D177" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E177" t="s">
         <v>2</v>
@@ -31116,10 +31113,10 @@
         <v>287</v>
       </c>
       <c r="C178" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D178" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E178" t="s">
         <v>2</v>
@@ -31127,16 +31124,16 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B179" t="s">
         <v>557</v>
       </c>
-      <c r="B179" t="s">
-        <v>558</v>
-      </c>
       <c r="C179" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D179" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E179" t="s">
         <v>2</v>
@@ -31144,16 +31141,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="B180" t="s">
         <v>559</v>
       </c>
-      <c r="B180" t="s">
-        <v>560</v>
-      </c>
       <c r="C180" t="s">
+        <v>375</v>
+      </c>
+      <c r="D180" t="s">
         <v>376</v>
-      </c>
-      <c r="D180" t="s">
-        <v>377</v>
       </c>
       <c r="E180" t="s">
         <v>2</v>
@@ -31161,16 +31158,16 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="B181" t="s">
         <v>561</v>
       </c>
-      <c r="B181" t="s">
-        <v>562</v>
-      </c>
       <c r="C181" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D181" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E181" t="s">
         <v>2</v>
@@ -31178,16 +31175,16 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
+        <v>562</v>
+      </c>
+      <c r="B182" t="s">
         <v>563</v>
       </c>
-      <c r="B182" t="s">
-        <v>564</v>
-      </c>
       <c r="C182" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D182" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E182" t="s">
         <v>2</v>
@@ -31201,10 +31198,10 @@
         <v>289</v>
       </c>
       <c r="C183" t="s">
+        <v>371</v>
+      </c>
+      <c r="D183" t="s">
         <v>372</v>
-      </c>
-      <c r="D183" t="s">
-        <v>373</v>
       </c>
       <c r="E183" t="s">
         <v>2</v>
@@ -31212,16 +31209,16 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B184" t="s">
         <v>565</v>
       </c>
-      <c r="B184" t="s">
-        <v>566</v>
-      </c>
       <c r="C184" t="s">
+        <v>384</v>
+      </c>
+      <c r="D184" t="s">
         <v>385</v>
-      </c>
-      <c r="D184" t="s">
-        <v>386</v>
       </c>
       <c r="E184" t="s">
         <v>2</v>
@@ -31229,16 +31226,16 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="B185" t="s">
         <v>567</v>
       </c>
-      <c r="B185" t="s">
-        <v>568</v>
-      </c>
       <c r="C185" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D185" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E185" t="s">
         <v>2</v>
@@ -31252,10 +31249,10 @@
         <v>205</v>
       </c>
       <c r="C186" t="s">
+        <v>375</v>
+      </c>
+      <c r="D186" t="s">
         <v>376</v>
-      </c>
-      <c r="D186" t="s">
-        <v>377</v>
       </c>
       <c r="E186" t="s">
         <v>2</v>
@@ -31263,16 +31260,16 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="B187" t="s">
         <v>569</v>
       </c>
-      <c r="B187" t="s">
-        <v>570</v>
-      </c>
       <c r="C187" t="s">
+        <v>375</v>
+      </c>
+      <c r="D187" t="s">
         <v>376</v>
-      </c>
-      <c r="D187" t="s">
-        <v>377</v>
       </c>
       <c r="E187" t="s">
         <v>2</v>
@@ -31280,16 +31277,16 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="B188" t="s">
         <v>571</v>
       </c>
-      <c r="B188" t="s">
-        <v>572</v>
-      </c>
       <c r="C188" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D188" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E188" t="s">
         <v>2</v>
@@ -31297,16 +31294,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="B189" t="s">
         <v>573</v>
       </c>
-      <c r="B189" t="s">
-        <v>574</v>
-      </c>
       <c r="C189" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D189" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E189" t="s">
         <v>2</v>
@@ -31320,10 +31317,10 @@
         <v>293</v>
       </c>
       <c r="C190" t="s">
+        <v>375</v>
+      </c>
+      <c r="D190" t="s">
         <v>376</v>
-      </c>
-      <c r="D190" t="s">
-        <v>377</v>
       </c>
       <c r="E190" t="s">
         <v>2</v>
@@ -31337,10 +31334,10 @@
         <v>319</v>
       </c>
       <c r="C191" t="s">
+        <v>371</v>
+      </c>
+      <c r="D191" t="s">
         <v>372</v>
-      </c>
-      <c r="D191" t="s">
-        <v>373</v>
       </c>
       <c r="E191" t="s">
         <v>2</v>
@@ -31348,16 +31345,16 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="B192" t="s">
         <v>575</v>
       </c>
-      <c r="B192" t="s">
-        <v>576</v>
-      </c>
       <c r="C192" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D192" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E192" t="s">
         <v>2</v>
@@ -31365,16 +31362,16 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="B193" t="s">
         <v>577</v>
       </c>
-      <c r="B193" t="s">
-        <v>578</v>
-      </c>
       <c r="C193" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D193" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E193" t="s">
         <v>2</v>
@@ -31382,16 +31379,16 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="B194" t="s">
         <v>579</v>
       </c>
-      <c r="B194" t="s">
-        <v>580</v>
-      </c>
       <c r="C194" t="s">
+        <v>377</v>
+      </c>
+      <c r="D194" t="s">
         <v>378</v>
-      </c>
-      <c r="D194" t="s">
-        <v>379</v>
       </c>
       <c r="E194" t="s">
         <v>2</v>
@@ -31405,10 +31402,10 @@
         <v>131</v>
       </c>
       <c r="C195" t="s">
+        <v>375</v>
+      </c>
+      <c r="D195" t="s">
         <v>376</v>
-      </c>
-      <c r="D195" t="s">
-        <v>377</v>
       </c>
       <c r="E195" t="s">
         <v>2</v>
@@ -31416,16 +31413,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="B196" t="s">
         <v>581</v>
       </c>
-      <c r="B196" t="s">
-        <v>582</v>
-      </c>
       <c r="C196" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D196" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E196" t="s">
         <v>2</v>
@@ -31439,10 +31436,10 @@
         <v>240</v>
       </c>
       <c r="C197" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D197" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E197" t="s">
         <v>2</v>
@@ -31456,10 +31453,10 @@
         <v>63</v>
       </c>
       <c r="C198" t="s">
+        <v>375</v>
+      </c>
+      <c r="D198" t="s">
         <v>376</v>
-      </c>
-      <c r="D198" t="s">
-        <v>377</v>
       </c>
       <c r="E198" t="s">
         <v>2</v>
@@ -31467,16 +31464,16 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="B199" t="s">
         <v>583</v>
       </c>
-      <c r="B199" t="s">
-        <v>584</v>
-      </c>
       <c r="C199" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D199" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E199" t="s">
         <v>2</v>
@@ -31490,10 +31487,10 @@
         <v>308</v>
       </c>
       <c r="C200" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D200" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E200" t="s">
         <v>2</v>
@@ -31501,16 +31498,16 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="B201" t="s">
         <v>585</v>
       </c>
-      <c r="B201" t="s">
-        <v>586</v>
-      </c>
       <c r="C201" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D201" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E201" t="s">
         <v>2</v>
@@ -31518,16 +31515,16 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="B202" t="s">
         <v>587</v>
       </c>
-      <c r="B202" t="s">
-        <v>588</v>
-      </c>
       <c r="C202" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D202" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E202" t="s">
         <v>2</v>
@@ -31541,10 +31538,10 @@
         <v>165</v>
       </c>
       <c r="C203" t="s">
+        <v>371</v>
+      </c>
+      <c r="D203" t="s">
         <v>372</v>
-      </c>
-      <c r="D203" t="s">
-        <v>373</v>
       </c>
       <c r="E203" t="s">
         <v>2</v>
@@ -31552,16 +31549,16 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="B204" t="s">
         <v>589</v>
       </c>
-      <c r="B204" t="s">
-        <v>590</v>
-      </c>
       <c r="C204" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D204" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E204" t="s">
         <v>2</v>
@@ -31569,16 +31566,16 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="B205" t="s">
         <v>591</v>
       </c>
-      <c r="B205" t="s">
-        <v>592</v>
-      </c>
       <c r="C205" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D205" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E205" t="s">
         <v>2</v>
@@ -31586,16 +31583,16 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="B206" t="s">
         <v>593</v>
       </c>
-      <c r="B206" t="s">
-        <v>594</v>
-      </c>
       <c r="C206" t="s">
+        <v>371</v>
+      </c>
+      <c r="D206" t="s">
         <v>372</v>
-      </c>
-      <c r="D206" t="s">
-        <v>373</v>
       </c>
       <c r="E206" t="s">
         <v>2</v>
@@ -31603,16 +31600,16 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="B207" t="s">
         <v>595</v>
       </c>
-      <c r="B207" t="s">
-        <v>596</v>
-      </c>
       <c r="C207" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D207" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E207" t="s">
         <v>2</v>
@@ -31626,10 +31623,10 @@
         <v>225</v>
       </c>
       <c r="C208" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D208" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E208" t="s">
         <v>2</v>
@@ -31643,10 +31640,10 @@
         <v>158</v>
       </c>
       <c r="C209" t="s">
+        <v>384</v>
+      </c>
+      <c r="D209" t="s">
         <v>385</v>
-      </c>
-      <c r="D209" t="s">
-        <v>386</v>
       </c>
       <c r="E209" t="s">
         <v>2</v>
@@ -31660,10 +31657,10 @@
         <v>166</v>
       </c>
       <c r="C210" t="s">
+        <v>377</v>
+      </c>
+      <c r="D210" t="s">
         <v>378</v>
-      </c>
-      <c r="D210" t="s">
-        <v>379</v>
       </c>
       <c r="E210" t="s">
         <v>2</v>
@@ -31674,13 +31671,13 @@
         <v>279</v>
       </c>
       <c r="B211" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C211" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D211" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E211" t="s">
         <v>2</v>
@@ -31688,16 +31685,16 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="B212" t="s">
         <v>598</v>
       </c>
-      <c r="B212" t="s">
-        <v>599</v>
-      </c>
       <c r="C212" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D212" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E212" t="s">
         <v>2</v>
@@ -31711,10 +31708,10 @@
         <v>259</v>
       </c>
       <c r="C213" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D213" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E213" t="s">
         <v>2</v>
@@ -31728,10 +31725,10 @@
         <v>330</v>
       </c>
       <c r="C214" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D214" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E214" t="s">
         <v>2</v>
@@ -31745,10 +31742,10 @@
         <v>247</v>
       </c>
       <c r="C215" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D215" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E215" t="s">
         <v>2</v>
@@ -31762,10 +31759,10 @@
         <v>256</v>
       </c>
       <c r="C216" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D216" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E216" t="s">
         <v>2</v>
@@ -31779,10 +31776,10 @@
         <v>133</v>
       </c>
       <c r="C217" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D217" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E217" t="s">
         <v>2</v>
@@ -31796,10 +31793,10 @@
         <v>316</v>
       </c>
       <c r="C218" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D218" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E218" t="s">
         <v>2</v>
@@ -31807,16 +31804,16 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="B219" t="s">
         <v>600</v>
       </c>
-      <c r="B219" t="s">
-        <v>601</v>
-      </c>
       <c r="C219" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D219" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E219" t="s">
         <v>2</v>
@@ -31830,10 +31827,10 @@
         <v>232</v>
       </c>
       <c r="C220" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D220" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E220" t="s">
         <v>2</v>
@@ -31847,10 +31844,10 @@
         <v>321</v>
       </c>
       <c r="C221" t="s">
+        <v>371</v>
+      </c>
+      <c r="D221" t="s">
         <v>372</v>
-      </c>
-      <c r="D221" t="s">
-        <v>373</v>
       </c>
       <c r="E221" t="s">
         <v>2</v>
@@ -31858,16 +31855,16 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="B222" t="s">
         <v>602</v>
       </c>
-      <c r="B222" t="s">
-        <v>603</v>
-      </c>
       <c r="C222" t="s">
+        <v>384</v>
+      </c>
+      <c r="D222" t="s">
         <v>385</v>
-      </c>
-      <c r="D222" t="s">
-        <v>386</v>
       </c>
       <c r="E222" t="s">
         <v>2</v>
@@ -31875,16 +31872,16 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="B223" t="s">
         <v>604</v>
       </c>
-      <c r="B223" t="s">
-        <v>605</v>
-      </c>
       <c r="C223" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D223" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E223" t="s">
         <v>2</v>
@@ -31892,16 +31889,16 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="B224" t="s">
         <v>606</v>
       </c>
-      <c r="B224" t="s">
-        <v>607</v>
-      </c>
       <c r="C224" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D224" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E224" t="s">
         <v>2</v>
@@ -31915,10 +31912,10 @@
         <v>155</v>
       </c>
       <c r="C225" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D225" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E225" t="s">
         <v>2</v>
@@ -31932,38 +31929,38 @@
         <v>358</v>
       </c>
       <c r="C226" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E226" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="B227" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="B227" s="5" t="s">
-        <v>609</v>
-      </c>
       <c r="C227" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E227" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="B228" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="B228" s="5" t="s">
-        <v>611</v>
-      </c>
       <c r="C228" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E228" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
@@ -31974,10 +31971,10 @@
         <v>363</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E229" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
@@ -31988,10 +31985,10 @@
         <v>365</v>
       </c>
       <c r="C230" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E230" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
@@ -32002,10 +31999,10 @@
         <v>364</v>
       </c>
       <c r="C231" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E231" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
@@ -32013,13 +32010,13 @@
         <v>244</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E232" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
@@ -32027,10 +32024,10 @@
         <v>194</v>
       </c>
       <c r="B233" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="F233" s="5" t="s">
         <v>613</v>
-      </c>
-      <c r="F233" s="5" t="s">
-        <v>614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial draft of week 8 activities
</commit_message>
<xml_diff>
--- a/src/tutorialpkg/data_db_activity/paralympics_all.xlsx
+++ b/src/tutorialpkg/data_db_activity/paralympics_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/comp0035-2024-tutorials/src/tutorialpkg/data_db_activity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9967DB-F9CE-D748-A176-35C2C6EDB219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160C547E-DCEE-1244-A223-2649FF3D7082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3827" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3827" uniqueCount="622">
   <si>
     <t>type</t>
   </si>
@@ -1140,9 +1140,6 @@
   </si>
   <si>
     <t>First summer games in France. The first time the Paralympic Opening Ceremony was held outside of a stadium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">winter </t>
   </si>
   <si>
     <t>Stoke Mandeville, New York</t>
@@ -2795,7 +2792,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2826,7 +2823,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -2850,7 +2847,7 @@
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -3137,10 +3134,10 @@
         <v>1984</v>
       </c>
       <c r="C8" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E8" s="1">
         <v>30850</v>
@@ -3677,7 +3674,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>367</v>
+        <v>62</v>
       </c>
       <c r="B20">
         <v>1976</v>
@@ -28083,36 +28080,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>620</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B2" t="s">
         <v>369</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>370</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>371</v>
-      </c>
-      <c r="D2" t="s">
-        <v>372</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -28120,16 +28117,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="B3" t="s">
         <v>373</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>374</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>375</v>
-      </c>
-      <c r="D3" t="s">
-        <v>376</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -28143,10 +28140,10 @@
         <v>242</v>
       </c>
       <c r="C4" t="s">
+        <v>376</v>
+      </c>
+      <c r="D4" t="s">
         <v>377</v>
-      </c>
-      <c r="D4" t="s">
-        <v>378</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -28154,16 +28151,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B5" t="s">
         <v>379</v>
       </c>
-      <c r="B5" t="s">
-        <v>380</v>
-      </c>
       <c r="C5" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5" t="s">
         <v>375</v>
-      </c>
-      <c r="D5" t="s">
-        <v>376</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -28177,10 +28174,10 @@
         <v>274</v>
       </c>
       <c r="C6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -28188,16 +28185,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B7" t="s">
         <v>382</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>383</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>384</v>
-      </c>
-      <c r="D7" t="s">
-        <v>385</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
@@ -28211,10 +28208,10 @@
         <v>134</v>
       </c>
       <c r="C8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D8" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E8" t="s">
         <v>2</v>
@@ -28222,16 +28219,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B9" t="s">
         <v>387</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" t="s">
         <v>388</v>
-      </c>
-      <c r="C9" t="s">
-        <v>375</v>
-      </c>
-      <c r="D9" t="s">
-        <v>389</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -28239,16 +28236,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B10" t="s">
         <v>390</v>
       </c>
-      <c r="B10" t="s">
-        <v>391</v>
-      </c>
       <c r="C10" t="s">
+        <v>383</v>
+      </c>
+      <c r="D10" t="s">
         <v>384</v>
-      </c>
-      <c r="D10" t="s">
-        <v>385</v>
       </c>
       <c r="E10" t="s">
         <v>2</v>
@@ -28256,16 +28253,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="B11" t="s">
         <v>392</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>393</v>
       </c>
-      <c r="C11" t="s">
-        <v>394</v>
-      </c>
       <c r="D11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E11" t="s">
         <v>2</v>
@@ -28279,10 +28276,10 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
@@ -28296,10 +28293,10 @@
         <v>69</v>
       </c>
       <c r="C13" t="s">
+        <v>374</v>
+      </c>
+      <c r="D13" t="s">
         <v>375</v>
-      </c>
-      <c r="D13" t="s">
-        <v>376</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
@@ -28313,10 +28310,10 @@
         <v>261</v>
       </c>
       <c r="C14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
@@ -28324,16 +28321,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B15" t="s">
         <v>395</v>
       </c>
-      <c r="B15" t="s">
-        <v>396</v>
-      </c>
       <c r="C15" t="s">
+        <v>383</v>
+      </c>
+      <c r="D15" t="s">
         <v>384</v>
-      </c>
-      <c r="D15" t="s">
-        <v>385</v>
       </c>
       <c r="E15" t="s">
         <v>2</v>
@@ -28341,16 +28338,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B16" t="s">
         <v>397</v>
       </c>
-      <c r="B16" t="s">
-        <v>398</v>
-      </c>
       <c r="C16" t="s">
+        <v>370</v>
+      </c>
+      <c r="D16" t="s">
         <v>371</v>
-      </c>
-      <c r="D16" t="s">
-        <v>372</v>
       </c>
       <c r="E16" t="s">
         <v>2</v>
@@ -28358,16 +28355,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B17" t="s">
         <v>399</v>
       </c>
-      <c r="B17" t="s">
-        <v>400</v>
-      </c>
       <c r="C17" t="s">
+        <v>383</v>
+      </c>
+      <c r="D17" t="s">
         <v>384</v>
-      </c>
-      <c r="D17" t="s">
-        <v>385</v>
       </c>
       <c r="E17" t="s">
         <v>2</v>
@@ -28375,16 +28372,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B18" t="s">
         <v>401</v>
       </c>
-      <c r="B18" t="s">
-        <v>402</v>
-      </c>
       <c r="C18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E18" t="s">
         <v>2</v>
@@ -28398,10 +28395,10 @@
         <v>136</v>
       </c>
       <c r="C19" t="s">
+        <v>374</v>
+      </c>
+      <c r="D19" t="s">
         <v>375</v>
-      </c>
-      <c r="D19" t="s">
-        <v>376</v>
       </c>
       <c r="E19" t="s">
         <v>2</v>
@@ -28409,16 +28406,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B20" t="s">
         <v>403</v>
       </c>
-      <c r="B20" t="s">
-        <v>404</v>
-      </c>
       <c r="C20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D20" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E20" t="s">
         <v>2</v>
@@ -28426,16 +28423,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B21" t="s">
         <v>405</v>
       </c>
-      <c r="B21" t="s">
-        <v>406</v>
-      </c>
       <c r="C21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E21" t="s">
         <v>2</v>
@@ -28443,16 +28440,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B22" t="s">
         <v>407</v>
       </c>
-      <c r="B22" t="s">
-        <v>408</v>
-      </c>
       <c r="C22" t="s">
+        <v>370</v>
+      </c>
+      <c r="D22" t="s">
         <v>371</v>
-      </c>
-      <c r="D22" t="s">
-        <v>372</v>
       </c>
       <c r="E22" t="s">
         <v>2</v>
@@ -28466,10 +28463,10 @@
         <v>263</v>
       </c>
       <c r="C23" t="s">
+        <v>374</v>
+      </c>
+      <c r="D23" t="s">
         <v>375</v>
-      </c>
-      <c r="D23" t="s">
-        <v>376</v>
       </c>
       <c r="E23" t="s">
         <v>2</v>
@@ -28477,16 +28474,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B24" t="s">
         <v>409</v>
       </c>
-      <c r="B24" t="s">
-        <v>410</v>
-      </c>
       <c r="C24" t="s">
+        <v>383</v>
+      </c>
+      <c r="D24" t="s">
         <v>384</v>
-      </c>
-      <c r="D24" t="s">
-        <v>385</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
@@ -28500,10 +28497,10 @@
         <v>236</v>
       </c>
       <c r="C25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D25" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E25" t="s">
         <v>2</v>
@@ -28511,16 +28508,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B26" t="s">
         <v>411</v>
       </c>
-      <c r="B26" t="s">
-        <v>412</v>
-      </c>
       <c r="C26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D26" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E26" t="s">
         <v>2</v>
@@ -28534,10 +28531,10 @@
         <v>280</v>
       </c>
       <c r="C27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D27" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
@@ -28551,10 +28548,10 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D28" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E28" t="s">
         <v>2</v>
@@ -28568,10 +28565,10 @@
         <v>160</v>
       </c>
       <c r="C29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D29" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E29" t="s">
         <v>2</v>
@@ -28579,16 +28576,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B30" t="s">
         <v>414</v>
       </c>
-      <c r="B30" t="s">
-        <v>415</v>
-      </c>
       <c r="C30" t="s">
+        <v>370</v>
+      </c>
+      <c r="D30" t="s">
         <v>371</v>
-      </c>
-      <c r="D30" t="s">
-        <v>372</v>
       </c>
       <c r="E30" t="s">
         <v>2</v>
@@ -28602,10 +28599,10 @@
         <v>162</v>
       </c>
       <c r="C31" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D31" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E31" t="s">
         <v>2</v>
@@ -28613,36 +28610,36 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B32" t="s">
         <v>416</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>376</v>
+      </c>
+      <c r="D32" t="s">
+        <v>380</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="5" t="s">
         <v>417</v>
-      </c>
-      <c r="C32" t="s">
-        <v>377</v>
-      </c>
-      <c r="D32" t="s">
-        <v>381</v>
-      </c>
-      <c r="E32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B33" t="s">
         <v>419</v>
       </c>
-      <c r="B33" t="s">
-        <v>420</v>
-      </c>
       <c r="C33" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D33" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E33" t="s">
         <v>2</v>
@@ -28650,16 +28647,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B34" t="s">
         <v>421</v>
       </c>
-      <c r="B34" t="s">
-        <v>422</v>
-      </c>
       <c r="C34" t="s">
+        <v>370</v>
+      </c>
+      <c r="D34" t="s">
         <v>371</v>
-      </c>
-      <c r="D34" t="s">
-        <v>372</v>
       </c>
       <c r="E34" t="s">
         <v>2</v>
@@ -28673,10 +28670,10 @@
         <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D35" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E35" t="s">
         <v>2</v>
@@ -28684,16 +28681,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B36" t="s">
         <v>423</v>
       </c>
-      <c r="B36" t="s">
-        <v>424</v>
-      </c>
       <c r="C36" t="s">
+        <v>383</v>
+      </c>
+      <c r="D36" t="s">
         <v>384</v>
-      </c>
-      <c r="D36" t="s">
-        <v>385</v>
       </c>
       <c r="E36" t="s">
         <v>2</v>
@@ -28701,36 +28698,36 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B37" t="s">
         <v>425</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
+        <v>376</v>
+      </c>
+      <c r="D37" t="s">
+        <v>380</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>426</v>
-      </c>
-      <c r="C37" t="s">
-        <v>377</v>
-      </c>
-      <c r="D37" t="s">
-        <v>381</v>
-      </c>
-      <c r="E37" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B38" t="s">
         <v>428</v>
       </c>
-      <c r="B38" t="s">
-        <v>429</v>
-      </c>
       <c r="C38" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D38" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E38" t="s">
         <v>2</v>
@@ -28744,10 +28741,10 @@
         <v>310</v>
       </c>
       <c r="C39" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D39" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E39" t="s">
         <v>2</v>
@@ -28761,10 +28758,10 @@
         <v>157</v>
       </c>
       <c r="C40" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D40" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E40" t="s">
         <v>2</v>
@@ -28775,13 +28772,13 @@
         <v>246</v>
       </c>
       <c r="B41" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C41" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D41" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E41" t="s">
         <v>2</v>
@@ -28789,16 +28786,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B42" t="s">
         <v>432</v>
       </c>
-      <c r="B42" t="s">
-        <v>433</v>
-      </c>
       <c r="C42" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D42" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E42" t="s">
         <v>2</v>
@@ -28806,16 +28803,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B43" t="s">
         <v>434</v>
       </c>
-      <c r="B43" t="s">
-        <v>435</v>
-      </c>
       <c r="C43" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D43" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E43" t="s">
         <v>2</v>
@@ -28823,16 +28820,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="B44" t="s">
         <v>436</v>
       </c>
-      <c r="B44" t="s">
-        <v>437</v>
-      </c>
       <c r="C44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D44" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E44" t="s">
         <v>2</v>
@@ -28846,10 +28843,10 @@
         <v>153</v>
       </c>
       <c r="C45" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D45" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E45" t="s">
         <v>2</v>
@@ -28857,16 +28854,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B46" t="s">
         <v>438</v>
       </c>
-      <c r="B46" t="s">
-        <v>439</v>
-      </c>
       <c r="C46" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D46" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E46" t="s">
         <v>2</v>
@@ -28880,10 +28877,10 @@
         <v>332</v>
       </c>
       <c r="C47" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D47" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E47" t="s">
         <v>2</v>
@@ -28897,10 +28894,10 @@
         <v>336</v>
       </c>
       <c r="C48" t="s">
+        <v>383</v>
+      </c>
+      <c r="D48" t="s">
         <v>384</v>
-      </c>
-      <c r="D48" t="s">
-        <v>385</v>
       </c>
       <c r="E48" t="s">
         <v>2</v>
@@ -28914,10 +28911,10 @@
         <v>227</v>
       </c>
       <c r="C49" t="s">
+        <v>374</v>
+      </c>
+      <c r="D49" t="s">
         <v>375</v>
-      </c>
-      <c r="D49" t="s">
-        <v>376</v>
       </c>
       <c r="E49" t="s">
         <v>2</v>
@@ -28931,10 +28928,10 @@
         <v>197</v>
       </c>
       <c r="C50" t="s">
+        <v>383</v>
+      </c>
+      <c r="D50" t="s">
         <v>384</v>
-      </c>
-      <c r="D50" t="s">
-        <v>385</v>
       </c>
       <c r="E50" t="s">
         <v>2</v>
@@ -28942,16 +28939,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B51" t="s">
         <v>440</v>
       </c>
-      <c r="B51" t="s">
-        <v>441</v>
-      </c>
       <c r="C51" t="s">
+        <v>383</v>
+      </c>
+      <c r="D51" t="s">
         <v>384</v>
-      </c>
-      <c r="D51" t="s">
-        <v>385</v>
       </c>
       <c r="E51" t="s">
         <v>2</v>
@@ -28965,10 +28962,10 @@
         <v>282</v>
       </c>
       <c r="C52" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D52" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E52" t="s">
         <v>2</v>
@@ -28982,16 +28979,16 @@
         <v>238</v>
       </c>
       <c r="C53" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D53" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E53" t="s">
         <v>2</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -29002,10 +28999,10 @@
         <v>149</v>
       </c>
       <c r="C54" t="s">
+        <v>374</v>
+      </c>
+      <c r="D54" t="s">
         <v>375</v>
-      </c>
-      <c r="D54" t="s">
-        <v>376</v>
       </c>
       <c r="E54" t="s">
         <v>2</v>
@@ -29013,16 +29010,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="B55" t="s">
         <v>443</v>
       </c>
-      <c r="B55" t="s">
-        <v>444</v>
-      </c>
       <c r="C55" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D55" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E55" t="s">
         <v>2</v>
@@ -29030,16 +29027,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="B56" t="s">
         <v>445</v>
       </c>
-      <c r="B56" t="s">
-        <v>446</v>
-      </c>
       <c r="C56" t="s">
+        <v>383</v>
+      </c>
+      <c r="D56" t="s">
         <v>384</v>
-      </c>
-      <c r="D56" t="s">
-        <v>385</v>
       </c>
       <c r="E56" t="s">
         <v>2</v>
@@ -29053,10 +29050,10 @@
         <v>249</v>
       </c>
       <c r="C57" t="s">
+        <v>383</v>
+      </c>
+      <c r="D57" t="s">
         <v>384</v>
-      </c>
-      <c r="D57" t="s">
-        <v>385</v>
       </c>
       <c r="E57" t="s">
         <v>2</v>
@@ -29070,10 +29067,10 @@
         <v>338</v>
       </c>
       <c r="C58" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D58" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E58" t="s">
         <v>2</v>
@@ -29087,10 +29084,10 @@
         <v>148</v>
       </c>
       <c r="C59" t="s">
+        <v>376</v>
+      </c>
+      <c r="D59" t="s">
         <v>377</v>
-      </c>
-      <c r="D59" t="s">
-        <v>378</v>
       </c>
       <c r="E59" t="s">
         <v>2</v>
@@ -29098,16 +29095,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="B60" t="s">
         <v>447</v>
       </c>
-      <c r="B60" t="s">
-        <v>448</v>
-      </c>
       <c r="C60" t="s">
+        <v>374</v>
+      </c>
+      <c r="D60" t="s">
         <v>375</v>
-      </c>
-      <c r="D60" t="s">
-        <v>376</v>
       </c>
       <c r="E60" t="s">
         <v>2</v>
@@ -29115,16 +29112,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="B61" t="s">
         <v>449</v>
       </c>
-      <c r="B61" t="s">
-        <v>450</v>
-      </c>
       <c r="C61" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D61" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E61" t="s">
         <v>2</v>
@@ -29138,10 +29135,10 @@
         <v>340</v>
       </c>
       <c r="C62" t="s">
+        <v>383</v>
+      </c>
+      <c r="D62" t="s">
         <v>384</v>
-      </c>
-      <c r="D62" t="s">
-        <v>385</v>
       </c>
       <c r="E62" t="s">
         <v>2</v>
@@ -29155,10 +29152,10 @@
         <v>38</v>
       </c>
       <c r="C63" t="s">
+        <v>374</v>
+      </c>
+      <c r="D63" t="s">
         <v>375</v>
-      </c>
-      <c r="D63" t="s">
-        <v>376</v>
       </c>
       <c r="E63" t="s">
         <v>2</v>
@@ -29172,10 +29169,10 @@
         <v>217</v>
       </c>
       <c r="C64" t="s">
+        <v>374</v>
+      </c>
+      <c r="D64" t="s">
         <v>375</v>
-      </c>
-      <c r="D64" t="s">
-        <v>376</v>
       </c>
       <c r="E64" t="s">
         <v>2</v>
@@ -29189,10 +29186,10 @@
         <v>314</v>
       </c>
       <c r="C65" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D65" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E65" t="s">
         <v>2</v>
@@ -29200,19 +29197,19 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="B66" t="s">
         <v>451</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>374</v>
+      </c>
+      <c r="D66" t="s">
+        <v>375</v>
+      </c>
+      <c r="E66" t="s">
         <v>452</v>
-      </c>
-      <c r="C66" t="s">
-        <v>375</v>
-      </c>
-      <c r="D66" t="s">
-        <v>376</v>
-      </c>
-      <c r="E66" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -29223,10 +29220,10 @@
         <v>357</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -29237,10 +29234,10 @@
         <v>312</v>
       </c>
       <c r="C68" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D68" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E68" t="s">
         <v>2</v>
@@ -29254,10 +29251,10 @@
         <v>137</v>
       </c>
       <c r="C69" t="s">
+        <v>374</v>
+      </c>
+      <c r="D69" t="s">
         <v>375</v>
-      </c>
-      <c r="D69" t="s">
-        <v>376</v>
       </c>
       <c r="E69" t="s">
         <v>2</v>
@@ -29271,10 +29268,10 @@
         <v>59</v>
       </c>
       <c r="C70" t="s">
+        <v>374</v>
+      </c>
+      <c r="D70" t="s">
         <v>375</v>
-      </c>
-      <c r="D70" t="s">
-        <v>376</v>
       </c>
       <c r="E70" t="s">
         <v>2</v>
@@ -29288,10 +29285,10 @@
         <v>163</v>
       </c>
       <c r="C71" t="s">
+        <v>374</v>
+      </c>
+      <c r="D71" t="s">
         <v>375</v>
-      </c>
-      <c r="D71" t="s">
-        <v>376</v>
       </c>
       <c r="E71" t="s">
         <v>2</v>
@@ -29299,16 +29296,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B72" t="s">
         <v>455</v>
       </c>
-      <c r="B72" t="s">
-        <v>456</v>
-      </c>
       <c r="C72" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D72" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E72" t="s">
         <v>2</v>
@@ -29316,16 +29313,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="B73" t="s">
         <v>457</v>
       </c>
-      <c r="B73" t="s">
-        <v>458</v>
-      </c>
       <c r="C73" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D73" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E73" t="s">
         <v>2</v>
@@ -29333,16 +29330,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="B74" t="s">
         <v>459</v>
       </c>
-      <c r="B74" t="s">
-        <v>460</v>
-      </c>
       <c r="C74" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D74" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E74" t="s">
         <v>2</v>
@@ -29356,10 +29353,10 @@
         <v>132</v>
       </c>
       <c r="C75" t="s">
+        <v>374</v>
+      </c>
+      <c r="D75" t="s">
         <v>375</v>
-      </c>
-      <c r="D75" t="s">
-        <v>376</v>
       </c>
       <c r="E75" t="s">
         <v>2</v>
@@ -29367,16 +29364,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="B76" t="s">
         <v>461</v>
       </c>
-      <c r="B76" t="s">
-        <v>462</v>
-      </c>
       <c r="C76" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D76" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E76" t="s">
         <v>2</v>
@@ -29390,10 +29387,10 @@
         <v>326</v>
       </c>
       <c r="C77" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D77" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E77" t="s">
         <v>2</v>
@@ -29401,16 +29398,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="B78" t="s">
         <v>463</v>
       </c>
-      <c r="B78" t="s">
-        <v>464</v>
-      </c>
       <c r="C78" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D78" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E78" t="s">
         <v>2</v>
@@ -29424,10 +29421,10 @@
         <v>24</v>
       </c>
       <c r="C79" t="s">
+        <v>374</v>
+      </c>
+      <c r="D79" t="s">
         <v>375</v>
-      </c>
-      <c r="D79" t="s">
-        <v>376</v>
       </c>
       <c r="E79" t="s">
         <v>2</v>
@@ -29435,16 +29432,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B80" t="s">
         <v>465</v>
       </c>
-      <c r="B80" t="s">
-        <v>466</v>
-      </c>
       <c r="C80" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D80" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E80" t="s">
         <v>2</v>
@@ -29452,16 +29449,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="B81" t="s">
         <v>467</v>
       </c>
-      <c r="B81" t="s">
-        <v>468</v>
-      </c>
       <c r="C81" t="s">
+        <v>383</v>
+      </c>
+      <c r="D81" t="s">
         <v>384</v>
-      </c>
-      <c r="D81" t="s">
-        <v>385</v>
       </c>
       <c r="E81" t="s">
         <v>2</v>
@@ -29475,10 +29472,10 @@
         <v>48</v>
       </c>
       <c r="C82" t="s">
+        <v>374</v>
+      </c>
+      <c r="D82" t="s">
         <v>375</v>
-      </c>
-      <c r="D82" t="s">
-        <v>376</v>
       </c>
       <c r="E82" t="s">
         <v>2</v>
@@ -29486,16 +29483,16 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="B83" t="s">
         <v>469</v>
       </c>
-      <c r="B83" t="s">
-        <v>470</v>
-      </c>
       <c r="C83" t="s">
+        <v>383</v>
+      </c>
+      <c r="D83" t="s">
         <v>384</v>
-      </c>
-      <c r="D83" t="s">
-        <v>385</v>
       </c>
       <c r="E83" t="s">
         <v>2</v>
@@ -29503,16 +29500,16 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="B84" t="s">
         <v>471</v>
       </c>
-      <c r="B84" t="s">
-        <v>472</v>
-      </c>
       <c r="C84" t="s">
+        <v>383</v>
+      </c>
+      <c r="D84" t="s">
         <v>384</v>
-      </c>
-      <c r="D84" t="s">
-        <v>385</v>
       </c>
       <c r="E84" t="s">
         <v>2</v>
@@ -29520,16 +29517,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="B85" t="s">
         <v>473</v>
       </c>
-      <c r="B85" t="s">
-        <v>474</v>
-      </c>
       <c r="C85" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D85" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E85" t="s">
         <v>2</v>
@@ -29537,16 +29534,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="B86" t="s">
         <v>475</v>
       </c>
-      <c r="B86" t="s">
-        <v>476</v>
-      </c>
       <c r="C86" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D86" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E86" t="s">
         <v>2</v>
@@ -29554,16 +29551,16 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="B87" t="s">
         <v>477</v>
       </c>
-      <c r="B87" t="s">
-        <v>478</v>
-      </c>
       <c r="C87" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D87" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E87" t="s">
         <v>2</v>
@@ -29571,16 +29568,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="B88" t="s">
         <v>479</v>
       </c>
-      <c r="B88" t="s">
-        <v>480</v>
-      </c>
       <c r="C88" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D88" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E88" t="s">
         <v>2</v>
@@ -29588,16 +29585,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B89" t="s">
         <v>481</v>
       </c>
-      <c r="B89" t="s">
-        <v>482</v>
-      </c>
       <c r="C89" t="s">
+        <v>383</v>
+      </c>
+      <c r="D89" t="s">
         <v>384</v>
-      </c>
-      <c r="D89" t="s">
-        <v>385</v>
       </c>
       <c r="E89" t="s">
         <v>2</v>
@@ -29611,10 +29608,10 @@
         <v>145</v>
       </c>
       <c r="C90" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D90" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E90" t="s">
         <v>2</v>
@@ -29622,16 +29619,16 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B91" t="s">
         <v>483</v>
       </c>
-      <c r="B91" t="s">
-        <v>484</v>
-      </c>
       <c r="C91" t="s">
+        <v>383</v>
+      </c>
+      <c r="D91" t="s">
         <v>384</v>
-      </c>
-      <c r="D91" t="s">
-        <v>385</v>
       </c>
       <c r="E91" t="s">
         <v>2</v>
@@ -29645,10 +29642,10 @@
         <v>146</v>
       </c>
       <c r="C92" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D92" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E92" t="s">
         <v>2</v>
@@ -29662,10 +29659,10 @@
         <v>150</v>
       </c>
       <c r="C93" t="s">
+        <v>370</v>
+      </c>
+      <c r="D93" t="s">
         <v>371</v>
-      </c>
-      <c r="D93" t="s">
-        <v>372</v>
       </c>
       <c r="E93" t="s">
         <v>2</v>
@@ -29679,10 +29676,10 @@
         <v>143</v>
       </c>
       <c r="C94" t="s">
+        <v>370</v>
+      </c>
+      <c r="D94" t="s">
         <v>371</v>
-      </c>
-      <c r="D94" t="s">
-        <v>372</v>
       </c>
       <c r="E94" t="s">
         <v>2</v>
@@ -29690,16 +29687,16 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B95" t="s">
         <v>485</v>
       </c>
-      <c r="B95" t="s">
-        <v>486</v>
-      </c>
       <c r="C95" t="s">
+        <v>374</v>
+      </c>
+      <c r="D95" t="s">
         <v>375</v>
-      </c>
-      <c r="D95" t="s">
-        <v>376</v>
       </c>
       <c r="E95" t="s">
         <v>2</v>
@@ -29707,22 +29704,22 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="B96" s="5" t="s">
         <v>487</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="C96" t="s">
+        <v>370</v>
+      </c>
+      <c r="D96" t="s">
+        <v>412</v>
+      </c>
+      <c r="E96" t="s">
         <v>488</v>
       </c>
-      <c r="C96" t="s">
-        <v>371</v>
-      </c>
-      <c r="D96" t="s">
-        <v>413</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="F96" s="5" t="s">
         <v>489</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -29733,10 +29730,10 @@
         <v>161</v>
       </c>
       <c r="C97" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D97" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E97" t="s">
         <v>2</v>
@@ -29750,10 +29747,10 @@
         <v>135</v>
       </c>
       <c r="C98" t="s">
+        <v>374</v>
+      </c>
+      <c r="D98" t="s">
         <v>375</v>
-      </c>
-      <c r="D98" t="s">
-        <v>376</v>
       </c>
       <c r="E98" t="s">
         <v>2</v>
@@ -29767,10 +29764,10 @@
         <v>229</v>
       </c>
       <c r="C99" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D99" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E99" t="s">
         <v>2</v>
@@ -29784,10 +29781,10 @@
         <v>154</v>
       </c>
       <c r="C100" t="s">
+        <v>374</v>
+      </c>
+      <c r="D100" t="s">
         <v>375</v>
-      </c>
-      <c r="D100" t="s">
-        <v>376</v>
       </c>
       <c r="E100" t="s">
         <v>2</v>
@@ -29801,10 +29798,10 @@
         <v>21</v>
       </c>
       <c r="C101" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D101" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E101" t="s">
         <v>2</v>
@@ -29812,16 +29809,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="B102" t="s">
         <v>491</v>
       </c>
-      <c r="B102" t="s">
-        <v>492</v>
-      </c>
       <c r="C102" t="s">
+        <v>383</v>
+      </c>
+      <c r="D102" t="s">
         <v>384</v>
-      </c>
-      <c r="D102" t="s">
-        <v>385</v>
       </c>
       <c r="E102" t="s">
         <v>2</v>
@@ -29835,10 +29832,10 @@
         <v>14</v>
       </c>
       <c r="C103" t="s">
+        <v>374</v>
+      </c>
+      <c r="D103" t="s">
         <v>375</v>
-      </c>
-      <c r="D103" t="s">
-        <v>376</v>
       </c>
       <c r="E103" t="s">
         <v>2</v>
@@ -29846,16 +29843,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="B104" t="s">
         <v>493</v>
       </c>
-      <c r="B104" t="s">
-        <v>494</v>
-      </c>
       <c r="C104" t="s">
+        <v>383</v>
+      </c>
+      <c r="D104" t="s">
         <v>384</v>
-      </c>
-      <c r="D104" t="s">
-        <v>385</v>
       </c>
       <c r="E104" t="s">
         <v>2</v>
@@ -29869,10 +29866,10 @@
         <v>139</v>
       </c>
       <c r="C105" t="s">
+        <v>383</v>
+      </c>
+      <c r="D105" t="s">
         <v>384</v>
-      </c>
-      <c r="D105" t="s">
-        <v>385</v>
       </c>
       <c r="E105" t="s">
         <v>2</v>
@@ -29886,10 +29883,10 @@
         <v>159</v>
       </c>
       <c r="C106" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D106" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E106" t="s">
         <v>2</v>
@@ -29903,10 +29900,10 @@
         <v>18</v>
       </c>
       <c r="C107" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D107" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E107" t="s">
         <v>2</v>
@@ -29920,10 +29917,10 @@
         <v>324</v>
       </c>
       <c r="C108" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D108" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E108" t="s">
         <v>2</v>
@@ -29937,10 +29934,10 @@
         <v>144</v>
       </c>
       <c r="C109" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D109" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E109" t="s">
         <v>2</v>
@@ -29948,16 +29945,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="B110" t="s">
         <v>495</v>
       </c>
-      <c r="B110" t="s">
-        <v>496</v>
-      </c>
       <c r="C110" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D110" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E110" t="s">
         <v>2</v>
@@ -29965,16 +29962,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="B111" t="s">
         <v>497</v>
       </c>
-      <c r="B111" t="s">
-        <v>498</v>
-      </c>
       <c r="C111" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D111" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E111" t="s">
         <v>2</v>
@@ -29988,10 +29985,10 @@
         <v>142</v>
       </c>
       <c r="C112" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D112" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E112" t="s">
         <v>2</v>
@@ -29999,16 +29996,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B113" t="s">
         <v>499</v>
       </c>
-      <c r="B113" t="s">
-        <v>500</v>
-      </c>
       <c r="C113" t="s">
+        <v>374</v>
+      </c>
+      <c r="D113" t="s">
         <v>375</v>
-      </c>
-      <c r="D113" t="s">
-        <v>376</v>
       </c>
       <c r="E113" t="s">
         <v>2</v>
@@ -30022,10 +30019,10 @@
         <v>355</v>
       </c>
       <c r="C114" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D114" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E114" t="s">
         <v>2</v>
@@ -30039,10 +30036,10 @@
         <v>152</v>
       </c>
       <c r="C115" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D115" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E115" t="s">
         <v>2</v>
@@ -30056,10 +30053,10 @@
         <v>304</v>
       </c>
       <c r="C116" t="s">
+        <v>370</v>
+      </c>
+      <c r="D116" t="s">
         <v>371</v>
-      </c>
-      <c r="D116" t="s">
-        <v>372</v>
       </c>
       <c r="E116" t="s">
         <v>2</v>
@@ -30073,10 +30070,10 @@
         <v>265</v>
       </c>
       <c r="C117" t="s">
+        <v>374</v>
+      </c>
+      <c r="D117" t="s">
         <v>375</v>
-      </c>
-      <c r="D117" t="s">
-        <v>376</v>
       </c>
       <c r="E117" t="s">
         <v>2</v>
@@ -30090,10 +30087,10 @@
         <v>267</v>
       </c>
       <c r="C118" t="s">
+        <v>376</v>
+      </c>
+      <c r="D118" t="s">
         <v>377</v>
-      </c>
-      <c r="D118" t="s">
-        <v>378</v>
       </c>
       <c r="E118" t="s">
         <v>2</v>
@@ -30107,10 +30104,10 @@
         <v>302</v>
       </c>
       <c r="C119" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D119" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E119" t="s">
         <v>2</v>
@@ -30118,16 +30115,16 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B120" t="s">
         <v>501</v>
       </c>
-      <c r="B120" t="s">
-        <v>502</v>
-      </c>
       <c r="C120" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D120" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E120" t="s">
         <v>2</v>
@@ -30135,16 +30132,16 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="B121" t="s">
         <v>503</v>
       </c>
-      <c r="B121" t="s">
-        <v>504</v>
-      </c>
       <c r="C121" t="s">
+        <v>383</v>
+      </c>
+      <c r="D121" t="s">
         <v>384</v>
-      </c>
-      <c r="D121" t="s">
-        <v>385</v>
       </c>
       <c r="E121" t="s">
         <v>2</v>
@@ -30152,16 +30149,16 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="B122" t="s">
         <v>505</v>
       </c>
-      <c r="B122" t="s">
-        <v>506</v>
-      </c>
       <c r="C122" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D122" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E122" t="s">
         <v>2</v>
@@ -30175,10 +30172,10 @@
         <v>349</v>
       </c>
       <c r="C123" t="s">
+        <v>374</v>
+      </c>
+      <c r="D123" t="s">
         <v>375</v>
-      </c>
-      <c r="D123" t="s">
-        <v>376</v>
       </c>
       <c r="E123" t="s">
         <v>2</v>
@@ -30192,10 +30189,10 @@
         <v>214</v>
       </c>
       <c r="C124" t="s">
+        <v>374</v>
+      </c>
+      <c r="D124" t="s">
         <v>375</v>
-      </c>
-      <c r="D124" t="s">
-        <v>376</v>
       </c>
       <c r="E124" t="s">
         <v>2</v>
@@ -30203,16 +30200,16 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="B125" t="s">
         <v>507</v>
       </c>
-      <c r="B125" t="s">
-        <v>508</v>
-      </c>
       <c r="C125" t="s">
+        <v>374</v>
+      </c>
+      <c r="D125" t="s">
         <v>375</v>
-      </c>
-      <c r="D125" t="s">
-        <v>376</v>
       </c>
       <c r="E125" t="s">
         <v>2</v>
@@ -30220,16 +30217,16 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="B126" t="s">
         <v>509</v>
       </c>
-      <c r="B126" t="s">
-        <v>510</v>
-      </c>
       <c r="C126" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D126" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E126" t="s">
         <v>2</v>
@@ -30237,16 +30234,16 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="B127" t="s">
         <v>511</v>
       </c>
-      <c r="B127" t="s">
-        <v>512</v>
-      </c>
       <c r="C127" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D127" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E127" t="s">
         <v>2</v>
@@ -30260,10 +30257,10 @@
         <v>168</v>
       </c>
       <c r="C128" t="s">
+        <v>376</v>
+      </c>
+      <c r="D128" t="s">
         <v>377</v>
-      </c>
-      <c r="D128" t="s">
-        <v>378</v>
       </c>
       <c r="E128" t="s">
         <v>2</v>
@@ -30277,10 +30274,10 @@
         <v>167</v>
       </c>
       <c r="C129" t="s">
+        <v>370</v>
+      </c>
+      <c r="D129" t="s">
         <v>371</v>
-      </c>
-      <c r="D129" t="s">
-        <v>372</v>
       </c>
       <c r="E129" t="s">
         <v>2</v>
@@ -30288,16 +30285,16 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B130" t="s">
         <v>513</v>
       </c>
-      <c r="B130" t="s">
-        <v>514</v>
-      </c>
       <c r="C130" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D130" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E130" t="s">
         <v>2</v>
@@ -30311,10 +30308,10 @@
         <v>254</v>
       </c>
       <c r="C131" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D131" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E131" t="s">
         <v>2</v>
@@ -30322,16 +30319,16 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="B132" t="s">
         <v>515</v>
       </c>
-      <c r="B132" t="s">
-        <v>516</v>
-      </c>
       <c r="C132" t="s">
+        <v>370</v>
+      </c>
+      <c r="D132" t="s">
         <v>371</v>
-      </c>
-      <c r="D132" t="s">
-        <v>372</v>
       </c>
       <c r="E132" t="s">
         <v>2</v>
@@ -30345,10 +30342,10 @@
         <v>147</v>
       </c>
       <c r="C133" t="s">
+        <v>383</v>
+      </c>
+      <c r="D133" t="s">
         <v>384</v>
-      </c>
-      <c r="D133" t="s">
-        <v>385</v>
       </c>
       <c r="E133" t="s">
         <v>2</v>
@@ -30362,10 +30359,10 @@
         <v>291</v>
       </c>
       <c r="C134" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D134" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E134" t="s">
         <v>2</v>
@@ -30373,16 +30370,16 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="B135" t="s">
         <v>517</v>
       </c>
-      <c r="B135" t="s">
-        <v>518</v>
-      </c>
       <c r="C135" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D135" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E135" t="s">
         <v>2</v>
@@ -30396,10 +30393,10 @@
         <v>284</v>
       </c>
       <c r="C136" t="s">
+        <v>374</v>
+      </c>
+      <c r="D136" t="s">
         <v>375</v>
-      </c>
-      <c r="D136" t="s">
-        <v>376</v>
       </c>
       <c r="E136" t="s">
         <v>2</v>
@@ -30407,16 +30404,16 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B137" t="s">
         <v>519</v>
       </c>
-      <c r="B137" t="s">
-        <v>520</v>
-      </c>
       <c r="C137" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D137" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E137" t="s">
         <v>2</v>
@@ -30424,16 +30421,16 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="B138" t="s">
         <v>521</v>
       </c>
-      <c r="B138" t="s">
-        <v>522</v>
-      </c>
       <c r="C138" t="s">
+        <v>374</v>
+      </c>
+      <c r="D138" t="s">
         <v>375</v>
-      </c>
-      <c r="D138" t="s">
-        <v>376</v>
       </c>
       <c r="E138" t="s">
         <v>2</v>
@@ -30447,10 +30444,10 @@
         <v>342</v>
       </c>
       <c r="C139" t="s">
+        <v>374</v>
+      </c>
+      <c r="D139" t="s">
         <v>375</v>
-      </c>
-      <c r="D139" t="s">
-        <v>376</v>
       </c>
       <c r="E139" t="s">
         <v>2</v>
@@ -30458,16 +30455,16 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="B140" t="s">
         <v>523</v>
       </c>
-      <c r="B140" t="s">
-        <v>524</v>
-      </c>
       <c r="C140" t="s">
+        <v>374</v>
+      </c>
+      <c r="D140" t="s">
         <v>375</v>
-      </c>
-      <c r="D140" t="s">
-        <v>376</v>
       </c>
       <c r="E140" t="s">
         <v>2</v>
@@ -30481,10 +30478,10 @@
         <v>334</v>
       </c>
       <c r="C141" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D141" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E141" t="s">
         <v>2</v>
@@ -30492,16 +30489,16 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="B142" t="s">
         <v>525</v>
       </c>
-      <c r="B142" t="s">
-        <v>526</v>
-      </c>
       <c r="C142" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D142" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E142" t="s">
         <v>2</v>
@@ -30509,16 +30506,16 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="B143" t="s">
         <v>527</v>
       </c>
-      <c r="B143" t="s">
-        <v>528</v>
-      </c>
       <c r="C143" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D143" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E143" t="s">
         <v>2</v>
@@ -30526,16 +30523,16 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="B144" t="s">
         <v>529</v>
       </c>
-      <c r="B144" t="s">
-        <v>530</v>
-      </c>
       <c r="C144" t="s">
+        <v>383</v>
+      </c>
+      <c r="D144" t="s">
         <v>384</v>
-      </c>
-      <c r="D144" t="s">
-        <v>385</v>
       </c>
       <c r="E144" t="s">
         <v>2</v>
@@ -30543,22 +30540,22 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="B145" t="s">
         <v>531</v>
       </c>
-      <c r="B145" t="s">
+      <c r="C145" t="s">
+        <v>370</v>
+      </c>
+      <c r="D145" t="s">
+        <v>371</v>
+      </c>
+      <c r="E145" t="s">
+        <v>2</v>
+      </c>
+      <c r="F145" s="5" t="s">
         <v>532</v>
-      </c>
-      <c r="C145" t="s">
-        <v>371</v>
-      </c>
-      <c r="D145" t="s">
-        <v>372</v>
-      </c>
-      <c r="E145" t="s">
-        <v>2</v>
-      </c>
-      <c r="F145" s="5" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -30569,10 +30566,10 @@
         <v>306</v>
       </c>
       <c r="C146" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D146" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E146" t="s">
         <v>2</v>
@@ -30580,16 +30577,16 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="B147" t="s">
         <v>534</v>
       </c>
-      <c r="B147" t="s">
-        <v>535</v>
-      </c>
       <c r="C147" t="s">
+        <v>383</v>
+      </c>
+      <c r="D147" t="s">
         <v>384</v>
-      </c>
-      <c r="D147" t="s">
-        <v>385</v>
       </c>
       <c r="E147" t="s">
         <v>2</v>
@@ -30597,16 +30594,16 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="B148" t="s">
         <v>536</v>
       </c>
-      <c r="B148" t="s">
-        <v>537</v>
-      </c>
       <c r="C148" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D148" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E148" t="s">
         <v>2</v>
@@ -30620,10 +30617,10 @@
         <v>31</v>
       </c>
       <c r="C149" t="s">
+        <v>374</v>
+      </c>
+      <c r="D149" t="s">
         <v>375</v>
-      </c>
-      <c r="D149" t="s">
-        <v>376</v>
       </c>
       <c r="E149" t="s">
         <v>2</v>
@@ -30631,16 +30628,16 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="B150" t="s">
         <v>538</v>
       </c>
-      <c r="B150" t="s">
-        <v>539</v>
-      </c>
       <c r="C150" t="s">
+        <v>370</v>
+      </c>
+      <c r="D150" t="s">
         <v>371</v>
-      </c>
-      <c r="D150" t="s">
-        <v>372</v>
       </c>
       <c r="E150" t="s">
         <v>2</v>
@@ -30654,10 +30651,10 @@
         <v>202</v>
       </c>
       <c r="C151" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D151" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E151" t="s">
         <v>2</v>
@@ -30665,16 +30662,16 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="B152" t="s">
         <v>540</v>
       </c>
-      <c r="B152" t="s">
-        <v>541</v>
-      </c>
       <c r="C152" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D152" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E152" t="s">
         <v>2</v>
@@ -30688,10 +30685,10 @@
         <v>66</v>
       </c>
       <c r="C153" t="s">
+        <v>374</v>
+      </c>
+      <c r="D153" t="s">
         <v>375</v>
-      </c>
-      <c r="D153" t="s">
-        <v>376</v>
       </c>
       <c r="E153" t="s">
         <v>2</v>
@@ -30705,27 +30702,27 @@
         <v>362</v>
       </c>
       <c r="C154" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D154" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E154" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="B155" t="s">
         <v>542</v>
       </c>
-      <c r="B155" t="s">
-        <v>543</v>
-      </c>
       <c r="C155" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D155" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E155" t="s">
         <v>2</v>
@@ -30739,10 +30736,10 @@
         <v>140</v>
       </c>
       <c r="C156" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D156" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E156" t="s">
         <v>2</v>
@@ -30756,10 +30753,10 @@
         <v>344</v>
       </c>
       <c r="C157" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D157" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E157" t="s">
         <v>2</v>
@@ -30773,10 +30770,10 @@
         <v>296</v>
       </c>
       <c r="C158" t="s">
+        <v>370</v>
+      </c>
+      <c r="D158" t="s">
         <v>371</v>
-      </c>
-      <c r="D158" t="s">
-        <v>372</v>
       </c>
       <c r="E158" t="s">
         <v>2</v>
@@ -30790,10 +30787,10 @@
         <v>210</v>
       </c>
       <c r="C159" t="s">
+        <v>383</v>
+      </c>
+      <c r="D159" t="s">
         <v>384</v>
-      </c>
-      <c r="D159" t="s">
-        <v>385</v>
       </c>
       <c r="E159" t="s">
         <v>2</v>
@@ -30801,16 +30798,16 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="B160" t="s">
         <v>544</v>
       </c>
-      <c r="B160" t="s">
-        <v>545</v>
-      </c>
       <c r="C160" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D160" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E160" t="s">
         <v>2</v>
@@ -30824,10 +30821,10 @@
         <v>151</v>
       </c>
       <c r="C161" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D161" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E161" t="s">
         <v>2</v>
@@ -30841,10 +30838,10 @@
         <v>271</v>
       </c>
       <c r="C162" t="s">
+        <v>370</v>
+      </c>
+      <c r="D162" t="s">
         <v>371</v>
-      </c>
-      <c r="D162" t="s">
-        <v>372</v>
       </c>
       <c r="E162" t="s">
         <v>2</v>
@@ -30858,10 +30855,10 @@
         <v>269</v>
       </c>
       <c r="C163" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D163" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E163" t="s">
         <v>2</v>
@@ -30869,16 +30866,16 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="B164" t="s">
         <v>546</v>
       </c>
-      <c r="B164" t="s">
-        <v>547</v>
-      </c>
       <c r="C164" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D164" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E164" t="s">
         <v>2</v>
@@ -30892,10 +30889,10 @@
         <v>298</v>
       </c>
       <c r="C165" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D165" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E165" t="s">
         <v>2</v>
@@ -30909,10 +30906,10 @@
         <v>141</v>
       </c>
       <c r="C166" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D166" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E166" t="s">
         <v>2</v>
@@ -30926,10 +30923,10 @@
         <v>156</v>
       </c>
       <c r="C167" t="s">
+        <v>374</v>
+      </c>
+      <c r="D167" t="s">
         <v>375</v>
-      </c>
-      <c r="D167" t="s">
-        <v>376</v>
       </c>
       <c r="E167" t="s">
         <v>2</v>
@@ -30937,16 +30934,16 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="B168" t="s">
         <v>548</v>
       </c>
-      <c r="B168" t="s">
-        <v>549</v>
-      </c>
       <c r="C168" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D168" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E168" t="s">
         <v>2</v>
@@ -30960,10 +30957,10 @@
         <v>164</v>
       </c>
       <c r="C169" t="s">
+        <v>383</v>
+      </c>
+      <c r="D169" t="s">
         <v>384</v>
-      </c>
-      <c r="D169" t="s">
-        <v>385</v>
       </c>
       <c r="E169" t="s">
         <v>2</v>
@@ -30971,16 +30968,16 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="B170" t="s">
         <v>550</v>
       </c>
-      <c r="B170" t="s">
-        <v>551</v>
-      </c>
       <c r="C170" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D170" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E170" t="s">
         <v>2</v>
@@ -30994,10 +30991,10 @@
         <v>328</v>
       </c>
       <c r="C171" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D171" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E171" t="s">
         <v>2</v>
@@ -31011,10 +31008,10 @@
         <v>300</v>
       </c>
       <c r="C172" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D172" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E172" t="s">
         <v>2</v>
@@ -31028,30 +31025,30 @@
         <v>354</v>
       </c>
       <c r="C173" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D173" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E173" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="B174" t="s">
         <v>552</v>
       </c>
-      <c r="B174" t="s">
-        <v>553</v>
-      </c>
       <c r="C174" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D174" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E174" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.2">
@@ -31062,10 +31059,10 @@
         <v>138</v>
       </c>
       <c r="C175" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D175" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E175" t="s">
         <v>2</v>
@@ -31073,19 +31070,19 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="B176" t="s">
         <v>554</v>
       </c>
-      <c r="B176" t="s">
-        <v>555</v>
-      </c>
       <c r="C176" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D176" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E176" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.2">
@@ -31096,10 +31093,10 @@
         <v>234</v>
       </c>
       <c r="C177" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D177" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E177" t="s">
         <v>2</v>
@@ -31113,10 +31110,10 @@
         <v>287</v>
       </c>
       <c r="C178" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D178" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E178" t="s">
         <v>2</v>
@@ -31124,16 +31121,16 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="B179" t="s">
         <v>556</v>
       </c>
-      <c r="B179" t="s">
-        <v>557</v>
-      </c>
       <c r="C179" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D179" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E179" t="s">
         <v>2</v>
@@ -31141,16 +31138,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="B180" t="s">
         <v>558</v>
       </c>
-      <c r="B180" t="s">
-        <v>559</v>
-      </c>
       <c r="C180" t="s">
+        <v>374</v>
+      </c>
+      <c r="D180" t="s">
         <v>375</v>
-      </c>
-      <c r="D180" t="s">
-        <v>376</v>
       </c>
       <c r="E180" t="s">
         <v>2</v>
@@ -31158,16 +31155,16 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="B181" t="s">
         <v>560</v>
       </c>
-      <c r="B181" t="s">
-        <v>561</v>
-      </c>
       <c r="C181" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D181" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E181" t="s">
         <v>2</v>
@@ -31175,16 +31172,16 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B182" t="s">
         <v>562</v>
       </c>
-      <c r="B182" t="s">
-        <v>563</v>
-      </c>
       <c r="C182" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D182" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E182" t="s">
         <v>2</v>
@@ -31198,10 +31195,10 @@
         <v>289</v>
       </c>
       <c r="C183" t="s">
+        <v>370</v>
+      </c>
+      <c r="D183" t="s">
         <v>371</v>
-      </c>
-      <c r="D183" t="s">
-        <v>372</v>
       </c>
       <c r="E183" t="s">
         <v>2</v>
@@ -31209,16 +31206,16 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="B184" t="s">
         <v>564</v>
       </c>
-      <c r="B184" t="s">
-        <v>565</v>
-      </c>
       <c r="C184" t="s">
+        <v>383</v>
+      </c>
+      <c r="D184" t="s">
         <v>384</v>
-      </c>
-      <c r="D184" t="s">
-        <v>385</v>
       </c>
       <c r="E184" t="s">
         <v>2</v>
@@ -31226,16 +31223,16 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B185" t="s">
         <v>566</v>
       </c>
-      <c r="B185" t="s">
-        <v>567</v>
-      </c>
       <c r="C185" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D185" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E185" t="s">
         <v>2</v>
@@ -31249,10 +31246,10 @@
         <v>205</v>
       </c>
       <c r="C186" t="s">
+        <v>374</v>
+      </c>
+      <c r="D186" t="s">
         <v>375</v>
-      </c>
-      <c r="D186" t="s">
-        <v>376</v>
       </c>
       <c r="E186" t="s">
         <v>2</v>
@@ -31260,16 +31257,16 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="B187" t="s">
         <v>568</v>
       </c>
-      <c r="B187" t="s">
-        <v>569</v>
-      </c>
       <c r="C187" t="s">
+        <v>374</v>
+      </c>
+      <c r="D187" t="s">
         <v>375</v>
-      </c>
-      <c r="D187" t="s">
-        <v>376</v>
       </c>
       <c r="E187" t="s">
         <v>2</v>
@@ -31277,16 +31274,16 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="B188" t="s">
         <v>570</v>
       </c>
-      <c r="B188" t="s">
-        <v>571</v>
-      </c>
       <c r="C188" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D188" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E188" t="s">
         <v>2</v>
@@ -31294,16 +31291,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="B189" t="s">
         <v>572</v>
       </c>
-      <c r="B189" t="s">
-        <v>573</v>
-      </c>
       <c r="C189" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D189" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E189" t="s">
         <v>2</v>
@@ -31317,10 +31314,10 @@
         <v>293</v>
       </c>
       <c r="C190" t="s">
+        <v>374</v>
+      </c>
+      <c r="D190" t="s">
         <v>375</v>
-      </c>
-      <c r="D190" t="s">
-        <v>376</v>
       </c>
       <c r="E190" t="s">
         <v>2</v>
@@ -31334,10 +31331,10 @@
         <v>319</v>
       </c>
       <c r="C191" t="s">
+        <v>370</v>
+      </c>
+      <c r="D191" t="s">
         <v>371</v>
-      </c>
-      <c r="D191" t="s">
-        <v>372</v>
       </c>
       <c r="E191" t="s">
         <v>2</v>
@@ -31345,16 +31342,16 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="B192" t="s">
         <v>574</v>
       </c>
-      <c r="B192" t="s">
-        <v>575</v>
-      </c>
       <c r="C192" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D192" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E192" t="s">
         <v>2</v>
@@ -31362,16 +31359,16 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="B193" t="s">
         <v>576</v>
       </c>
-      <c r="B193" t="s">
-        <v>577</v>
-      </c>
       <c r="C193" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D193" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E193" t="s">
         <v>2</v>
@@ -31379,16 +31376,16 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="B194" t="s">
         <v>578</v>
       </c>
-      <c r="B194" t="s">
-        <v>579</v>
-      </c>
       <c r="C194" t="s">
+        <v>376</v>
+      </c>
+      <c r="D194" t="s">
         <v>377</v>
-      </c>
-      <c r="D194" t="s">
-        <v>378</v>
       </c>
       <c r="E194" t="s">
         <v>2</v>
@@ -31402,10 +31399,10 @@
         <v>131</v>
       </c>
       <c r="C195" t="s">
+        <v>374</v>
+      </c>
+      <c r="D195" t="s">
         <v>375</v>
-      </c>
-      <c r="D195" t="s">
-        <v>376</v>
       </c>
       <c r="E195" t="s">
         <v>2</v>
@@ -31413,16 +31410,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="B196" t="s">
         <v>580</v>
       </c>
-      <c r="B196" t="s">
-        <v>581</v>
-      </c>
       <c r="C196" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D196" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E196" t="s">
         <v>2</v>
@@ -31436,10 +31433,10 @@
         <v>240</v>
       </c>
       <c r="C197" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D197" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E197" t="s">
         <v>2</v>
@@ -31453,10 +31450,10 @@
         <v>63</v>
       </c>
       <c r="C198" t="s">
+        <v>374</v>
+      </c>
+      <c r="D198" t="s">
         <v>375</v>
-      </c>
-      <c r="D198" t="s">
-        <v>376</v>
       </c>
       <c r="E198" t="s">
         <v>2</v>
@@ -31464,16 +31461,16 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="B199" t="s">
         <v>582</v>
       </c>
-      <c r="B199" t="s">
-        <v>583</v>
-      </c>
       <c r="C199" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D199" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E199" t="s">
         <v>2</v>
@@ -31487,10 +31484,10 @@
         <v>308</v>
       </c>
       <c r="C200" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D200" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E200" t="s">
         <v>2</v>
@@ -31498,16 +31495,16 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="B201" t="s">
         <v>584</v>
       </c>
-      <c r="B201" t="s">
-        <v>585</v>
-      </c>
       <c r="C201" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D201" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E201" t="s">
         <v>2</v>
@@ -31515,16 +31512,16 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="B202" t="s">
         <v>586</v>
       </c>
-      <c r="B202" t="s">
-        <v>587</v>
-      </c>
       <c r="C202" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D202" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E202" t="s">
         <v>2</v>
@@ -31538,10 +31535,10 @@
         <v>165</v>
       </c>
       <c r="C203" t="s">
+        <v>370</v>
+      </c>
+      <c r="D203" t="s">
         <v>371</v>
-      </c>
-      <c r="D203" t="s">
-        <v>372</v>
       </c>
       <c r="E203" t="s">
         <v>2</v>
@@ -31549,16 +31546,16 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="B204" t="s">
         <v>588</v>
       </c>
-      <c r="B204" t="s">
-        <v>589</v>
-      </c>
       <c r="C204" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D204" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E204" t="s">
         <v>2</v>
@@ -31566,16 +31563,16 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="B205" t="s">
         <v>590</v>
       </c>
-      <c r="B205" t="s">
-        <v>591</v>
-      </c>
       <c r="C205" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D205" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E205" t="s">
         <v>2</v>
@@ -31583,16 +31580,16 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="B206" t="s">
         <v>592</v>
       </c>
-      <c r="B206" t="s">
-        <v>593</v>
-      </c>
       <c r="C206" t="s">
+        <v>370</v>
+      </c>
+      <c r="D206" t="s">
         <v>371</v>
-      </c>
-      <c r="D206" t="s">
-        <v>372</v>
       </c>
       <c r="E206" t="s">
         <v>2</v>
@@ -31600,16 +31597,16 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="B207" t="s">
         <v>594</v>
       </c>
-      <c r="B207" t="s">
-        <v>595</v>
-      </c>
       <c r="C207" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D207" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E207" t="s">
         <v>2</v>
@@ -31623,10 +31620,10 @@
         <v>225</v>
       </c>
       <c r="C208" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D208" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E208" t="s">
         <v>2</v>
@@ -31640,10 +31637,10 @@
         <v>158</v>
       </c>
       <c r="C209" t="s">
+        <v>383</v>
+      </c>
+      <c r="D209" t="s">
         <v>384</v>
-      </c>
-      <c r="D209" t="s">
-        <v>385</v>
       </c>
       <c r="E209" t="s">
         <v>2</v>
@@ -31657,10 +31654,10 @@
         <v>166</v>
       </c>
       <c r="C210" t="s">
+        <v>376</v>
+      </c>
+      <c r="D210" t="s">
         <v>377</v>
-      </c>
-      <c r="D210" t="s">
-        <v>378</v>
       </c>
       <c r="E210" t="s">
         <v>2</v>
@@ -31671,13 +31668,13 @@
         <v>279</v>
       </c>
       <c r="B211" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C211" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D211" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E211" t="s">
         <v>2</v>
@@ -31685,16 +31682,16 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="B212" t="s">
         <v>597</v>
       </c>
-      <c r="B212" t="s">
-        <v>598</v>
-      </c>
       <c r="C212" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D212" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E212" t="s">
         <v>2</v>
@@ -31708,10 +31705,10 @@
         <v>259</v>
       </c>
       <c r="C213" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D213" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E213" t="s">
         <v>2</v>
@@ -31725,10 +31722,10 @@
         <v>330</v>
       </c>
       <c r="C214" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D214" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E214" t="s">
         <v>2</v>
@@ -31742,10 +31739,10 @@
         <v>247</v>
       </c>
       <c r="C215" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D215" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E215" t="s">
         <v>2</v>
@@ -31759,10 +31756,10 @@
         <v>256</v>
       </c>
       <c r="C216" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D216" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E216" t="s">
         <v>2</v>
@@ -31776,10 +31773,10 @@
         <v>133</v>
       </c>
       <c r="C217" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D217" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E217" t="s">
         <v>2</v>
@@ -31793,10 +31790,10 @@
         <v>316</v>
       </c>
       <c r="C218" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D218" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E218" t="s">
         <v>2</v>
@@ -31804,16 +31801,16 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B219" t="s">
         <v>599</v>
       </c>
-      <c r="B219" t="s">
-        <v>600</v>
-      </c>
       <c r="C219" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D219" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E219" t="s">
         <v>2</v>
@@ -31827,10 +31824,10 @@
         <v>232</v>
       </c>
       <c r="C220" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D220" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E220" t="s">
         <v>2</v>
@@ -31844,10 +31841,10 @@
         <v>321</v>
       </c>
       <c r="C221" t="s">
+        <v>370</v>
+      </c>
+      <c r="D221" t="s">
         <v>371</v>
-      </c>
-      <c r="D221" t="s">
-        <v>372</v>
       </c>
       <c r="E221" t="s">
         <v>2</v>
@@ -31855,16 +31852,16 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="B222" t="s">
         <v>601</v>
       </c>
-      <c r="B222" t="s">
-        <v>602</v>
-      </c>
       <c r="C222" t="s">
+        <v>383</v>
+      </c>
+      <c r="D222" t="s">
         <v>384</v>
-      </c>
-      <c r="D222" t="s">
-        <v>385</v>
       </c>
       <c r="E222" t="s">
         <v>2</v>
@@ -31872,16 +31869,16 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="B223" t="s">
         <v>603</v>
       </c>
-      <c r="B223" t="s">
-        <v>604</v>
-      </c>
       <c r="C223" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D223" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E223" t="s">
         <v>2</v>
@@ -31889,16 +31886,16 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="B224" t="s">
         <v>605</v>
       </c>
-      <c r="B224" t="s">
-        <v>606</v>
-      </c>
       <c r="C224" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D224" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E224" t="s">
         <v>2</v>
@@ -31912,10 +31909,10 @@
         <v>155</v>
       </c>
       <c r="C225" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D225" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E225" t="s">
         <v>2</v>
@@ -31929,38 +31926,38 @@
         <v>358</v>
       </c>
       <c r="C226" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E226" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="B227" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="B227" s="5" t="s">
-        <v>608</v>
-      </c>
       <c r="C227" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E227" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="B228" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="B228" s="5" t="s">
-        <v>610</v>
-      </c>
       <c r="C228" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E228" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
@@ -31971,10 +31968,10 @@
         <v>363</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E229" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
@@ -31985,10 +31982,10 @@
         <v>365</v>
       </c>
       <c r="C230" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E230" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
@@ -31999,10 +31996,10 @@
         <v>364</v>
       </c>
       <c r="C231" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E231" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
@@ -32010,13 +32007,13 @@
         <v>244</v>
       </c>
       <c r="B232" s="5" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C232" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E232" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
@@ -32024,10 +32021,10 @@
         <v>194</v>
       </c>
       <c r="B233" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="F233" s="5" t="s">
         <v>612</v>
-      </c>
-      <c r="F233" s="5" t="s">
-        <v>613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>